<commit_message>
1b_child_counts_and_census.qmd --- cleaned up the chi-square (w/o residuals) again
</commit_message>
<xml_diff>
--- a/Data/use_this_replacement_racial_group_representation.xlsx
+++ b/Data/use_this_replacement_racial_group_representation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEED508-F10E-9942-98E8-F22BF5FA8714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9708A837-8E89-4643-B06A-803417DE10FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="500" windowWidth="16280" windowHeight="15920" activeTab="1" xr2:uid="{4D43684D-767A-5B42-8EFD-CDAF7BC426E6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" activeTab="2" xr2:uid="{4D43684D-767A-5B42-8EFD-CDAF7BC426E6}"/>
   </bookViews>
   <sheets>
     <sheet name="2020 national CC vs census" sheetId="4" r:id="rId1"/>
@@ -571,7 +571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -714,6 +714,22 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -758,26 +774,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3668,8 +3664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB304EA7-6C1E-224C-AD55-AA784971FFF0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3681,15 +3677,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1A8275-12E4-4647-8849-23CE8825B359}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="A1:H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="56" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="56" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>55</v>
       </c>
@@ -3715,59 +3711,67 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="83" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="81" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="84">
+      <c r="B2" s="66">
         <v>212000</v>
       </c>
-      <c r="C2" s="82">
+      <c r="C2" s="65">
         <v>674000</v>
       </c>
-      <c r="D2" s="82">
+      <c r="D2" s="65">
         <v>1799000</v>
       </c>
-      <c r="E2" s="82">
+      <c r="E2" s="65">
         <v>2953000</v>
       </c>
-      <c r="F2" s="84">
+      <c r="F2" s="66">
         <v>42000</v>
       </c>
-      <c r="G2" s="82">
+      <c r="G2" s="65">
         <v>738000</v>
       </c>
-      <c r="H2" s="82">
+      <c r="H2" s="65">
         <v>7895000</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="80" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="77" t="s">
+      <c r="J2" s="67"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="78">
+      <c r="B3" s="63">
         <v>5842</v>
       </c>
-      <c r="C3" s="78">
+      <c r="C3" s="63">
         <v>36966</v>
       </c>
-      <c r="D3" s="78">
+      <c r="D3" s="63">
         <v>104046</v>
       </c>
-      <c r="E3" s="78">
+      <c r="E3" s="63">
         <v>232969</v>
       </c>
-      <c r="F3" s="78">
+      <c r="F3" s="63">
         <v>2557</v>
       </c>
-      <c r="G3" s="78">
+      <c r="G3" s="63">
         <v>35650</v>
       </c>
-      <c r="H3" s="79">
+      <c r="H3" s="64">
         <v>424383</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J4" s="67"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J5" s="22"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -3776,6 +3780,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3798,18 +3803,18 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="82">
+      <c r="B2" s="65">
         <v>2953000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="78">
+      <c r="B3" s="63">
         <v>232969</v>
       </c>
     </row>
@@ -4044,44 +4049,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="65">
+      <c r="B1" s="71">
         <v>2020</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="63"/>
-      <c r="B2" s="67" t="s">
+      <c r="A2" s="69"/>
+      <c r="B2" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="71" t="s">
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="73" t="s">
+      <c r="J2" s="79" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="102" x14ac:dyDescent="0.2">
-      <c r="A3" s="64"/>
-      <c r="B3" s="68"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="74"/>
       <c r="C3" s="8" t="s">
         <v>14</v>
       </c>
@@ -4100,8 +4105,8 @@
       <c r="H3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="72"/>
-      <c r="J3" s="74"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="80"/>
       <c r="K3" s="14" t="s">
         <v>23</v>
       </c>
@@ -4824,44 +4829,44 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="65">
+      <c r="B7" s="71">
         <v>2020</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="66"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
     </row>
     <row r="8" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="63"/>
-      <c r="B8" s="67" t="s">
+      <c r="A8" s="69"/>
+      <c r="B8" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="65" t="s">
+      <c r="D8" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="71" t="s">
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="75"/>
+      <c r="I8" s="76"/>
+      <c r="J8" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="81" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="102" x14ac:dyDescent="0.2">
-      <c r="A9" s="64"/>
-      <c r="B9" s="68"/>
+      <c r="A9" s="70"/>
+      <c r="B9" s="74"/>
       <c r="C9" t="s">
         <v>36</v>
       </c>
@@ -4883,8 +4888,8 @@
       <c r="I9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="72"/>
-      <c r="K9" s="76"/>
+      <c r="J9" s="78"/>
+      <c r="K9" s="82"/>
       <c r="L9" s="14" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
1b_child_coutns_and_census.qmd --- remvoed Hispanic from comparisons, updated tables, chi-square w. residuals, trying to do OR too.
</commit_message>
<xml_diff>
--- a/Data/use_this_replacement_racial_group_representation.xlsx
+++ b/Data/use_this_replacement_racial_group_representation.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9708A837-8E89-4643-B06A-803417DE10FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1CBE25-D116-414F-A985-F19D9CF52FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" activeTab="2" xr2:uid="{4D43684D-767A-5B42-8EFD-CDAF7BC426E6}"/>
+    <workbookView xWindow="4980" yWindow="680" windowWidth="19280" windowHeight="14880" firstSheet="3" activeTab="8" xr2:uid="{4D43684D-767A-5B42-8EFD-CDAF7BC426E6}"/>
   </bookViews>
   <sheets>
     <sheet name="2020 national CC vs census" sheetId="4" r:id="rId1"/>
-    <sheet name="2020 national CC vs census char" sheetId="8" r:id="rId2"/>
+    <sheet name="2020 national CC vs census cha1" sheetId="8" r:id="rId2"/>
     <sheet name="2020 national cc vs census numb" sheetId="10" r:id="rId3"/>
-    <sheet name="2020 census vs cc hispanic" sheetId="9" r:id="rId4"/>
-    <sheet name="2020 Child Count" sheetId="1" r:id="rId5"/>
-    <sheet name="2020 Census count" sheetId="2" r:id="rId6"/>
-    <sheet name="2020 census basic table for res" sheetId="6" r:id="rId7"/>
-    <sheet name="2020 % based on census" sheetId="3" r:id="rId8"/>
-    <sheet name="Oregon CC vs census " sheetId="5" r:id="rId9"/>
+    <sheet name="2020 national cc vs cen num2 ch" sheetId="12" r:id="rId4"/>
+    <sheet name="2020 national CC vs census num2" sheetId="11" r:id="rId5"/>
+    <sheet name="2020 census vs cc hispanic" sheetId="9" r:id="rId6"/>
+    <sheet name="2020 Child Count" sheetId="1" r:id="rId7"/>
+    <sheet name="2020 Census count" sheetId="2" r:id="rId8"/>
+    <sheet name="2020 census basic table for res" sheetId="6" r:id="rId9"/>
+    <sheet name="2020 % based on census" sheetId="3" r:id="rId10"/>
+    <sheet name="Oregon CC vs census " sheetId="5" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="59">
   <si>
     <t>State</t>
   </si>
@@ -252,6 +254,9 @@
   </si>
   <si>
     <t>EI Population</t>
+  </si>
+  <si>
+    <t>Total - Hispanic</t>
   </si>
 </sst>
 </file>
@@ -571,7 +576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -730,6 +735,15 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -775,6 +789,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3566,15 +3581,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7207DC-21F2-074F-A16E-82DD5230C551}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="56" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="56" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
@@ -3597,7 +3616,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -3623,7 +3642,7 @@
         <v>0.55151938526021704</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -3649,14 +3668,764 @@
         <v>0.50377071578904886</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C6" s="20" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="56" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="68" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="66">
+        <v>212000</v>
+      </c>
+      <c r="C12" s="66">
+        <v>674000</v>
+      </c>
+      <c r="D12" s="66">
+        <v>1799000</v>
+      </c>
+      <c r="E12" s="66">
+        <v>2953000</v>
+      </c>
+      <c r="F12" s="66">
+        <v>42000</v>
+      </c>
+      <c r="G12" s="66">
+        <v>738000</v>
+      </c>
+      <c r="H12" s="66">
+        <v>7895000</v>
+      </c>
+      <c r="I12" s="67">
+        <v>14313000</v>
+      </c>
+      <c r="J12" s="67">
+        <v>11360000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="62"/>
+      <c r="B13" s="66">
+        <f>B12/J12</f>
+        <v>1.8661971830985915E-2</v>
+      </c>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65">
+        <f>H12/J12</f>
+        <v>0.69498239436619713</v>
+      </c>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="69">
+        <v>5842</v>
+      </c>
+      <c r="C14" s="69">
+        <v>36966</v>
+      </c>
+      <c r="D14" s="69">
+        <v>104046</v>
+      </c>
+      <c r="E14" s="69">
+        <v>232969</v>
+      </c>
+      <c r="F14" s="69">
+        <v>2557</v>
+      </c>
+      <c r="G14" s="69">
+        <v>35650</v>
+      </c>
+      <c r="H14" s="70">
+        <v>424383</v>
+      </c>
+      <c r="I14" s="67">
+        <f>SUM(B14:H14)</f>
+        <v>842413</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <f>H14/I14</f>
+        <v>0.50377071578904886</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE57A53-26B7-CD40-AFB1-B8A430F77433}">
+  <dimension ref="A1:M23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="56" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>1.4809640237513098E-2</v>
+      </c>
+      <c r="C2">
+        <v>4.7083478868319942E-2</v>
+      </c>
+      <c r="D2">
+        <v>0.12567237163814182</v>
+      </c>
+      <c r="E2">
+        <v>0.20628711142158576</v>
+      </c>
+      <c r="F2">
+        <v>2.9339853300733498E-3</v>
+      </c>
+      <c r="G2">
+        <v>5.1554313657003144E-2</v>
+      </c>
+      <c r="H2">
+        <v>0.55151938526021704</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>6.9348407491337388E-3</v>
+      </c>
+      <c r="C3">
+        <v>4.3881089204463847E-2</v>
+      </c>
+      <c r="D3">
+        <v>0.12350949000074785</v>
+      </c>
+      <c r="E3">
+        <v>0.27654962589608661</v>
+      </c>
+      <c r="F3">
+        <v>3.0353282772226926E-3</v>
+      </c>
+      <c r="G3">
+        <v>4.2318910083296433E-2</v>
+      </c>
+      <c r="H3">
+        <v>0.50377071578904886</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="71" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="74">
+        <v>2020</v>
+      </c>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+    </row>
+    <row r="8" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="72"/>
+      <c r="B8" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="79"/>
+      <c r="J8" s="80" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="84" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+      <c r="A9" s="73"/>
+      <c r="B9" s="77"/>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="81"/>
+      <c r="K9" s="85"/>
+      <c r="L9" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="12">
+        <v>3735</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="13">
+        <v>2597</v>
+      </c>
+      <c r="E10" s="13">
+        <v>591</v>
+      </c>
+      <c r="F10" s="13">
+        <v>70</v>
+      </c>
+      <c r="G10" s="13">
+        <v>217</v>
+      </c>
+      <c r="H10" s="13">
+        <v>14</v>
+      </c>
+      <c r="I10" s="12">
+        <v>246</v>
+      </c>
+      <c r="J10" s="13">
+        <v>970</v>
+      </c>
+      <c r="K10" s="15">
+        <v>1807</v>
+      </c>
+      <c r="L10" s="5">
+        <f>SUM(J10:K10)</f>
+        <v>2777</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="12">
+        <v>3774</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="13">
+        <v>2623</v>
+      </c>
+      <c r="E11" s="13">
+        <v>598</v>
+      </c>
+      <c r="F11" s="13">
+        <v>71</v>
+      </c>
+      <c r="G11" s="13">
+        <v>223</v>
+      </c>
+      <c r="H11" s="13">
+        <v>14</v>
+      </c>
+      <c r="I11" s="12">
+        <v>244</v>
+      </c>
+      <c r="J11" s="13">
+        <v>986</v>
+      </c>
+      <c r="K11" s="15">
+        <v>1819</v>
+      </c>
+      <c r="L11" s="5">
+        <f t="shared" ref="L11:L12" si="0">SUM(J11:K11)</f>
+        <v>2805</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="12">
+        <v>3853</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="13">
+        <v>2675</v>
+      </c>
+      <c r="E12" s="13">
+        <v>610</v>
+      </c>
+      <c r="F12" s="13">
+        <v>71</v>
+      </c>
+      <c r="G12" s="13">
+        <v>234</v>
+      </c>
+      <c r="H12" s="13">
+        <v>14</v>
+      </c>
+      <c r="I12" s="12">
+        <v>248</v>
+      </c>
+      <c r="J12" s="13">
+        <v>997</v>
+      </c>
+      <c r="K12" s="15">
+        <v>1859</v>
+      </c>
+      <c r="L12" s="5">
+        <f t="shared" si="0"/>
+        <v>2856</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B13" s="5">
+        <f>SUM(B10:B12)</f>
+        <v>11362</v>
+      </c>
+      <c r="C13" s="5">
+        <v>19800</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" ref="D13:L13" si="1">SUM(D10:D12)</f>
+        <v>7895</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>1799</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="1"/>
+        <v>212</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="1"/>
+        <v>674</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" si="1"/>
+        <v>738</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" si="1"/>
+        <v>2953</v>
+      </c>
+      <c r="K13" s="16">
+        <f t="shared" si="1"/>
+        <v>5485</v>
+      </c>
+      <c r="L13" s="5">
+        <f t="shared" si="1"/>
+        <v>8438</v>
+      </c>
+      <c r="M13" s="5">
+        <f>SUM(B13+L13)</f>
+        <v>19800</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="5">
+        <v>5485</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="5">
+        <v>13380</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17">
+        <v>0.55151938526021704</v>
+      </c>
+      <c r="E16" s="17">
+        <f>E13/C13</f>
+        <v>9.0858585858585861E-2</v>
+      </c>
+      <c r="F16" s="17">
+        <f>F13/C13</f>
+        <v>1.0707070707070707E-2</v>
+      </c>
+      <c r="G16" s="17">
+        <f>G13/C13</f>
+        <v>3.4040404040404038E-2</v>
+      </c>
+      <c r="H16" s="17">
+        <f>H13/C13</f>
+        <v>2.1212121212121214E-3</v>
+      </c>
+      <c r="I16" s="17">
+        <f>I13/C13</f>
+        <v>3.727272727272727E-2</v>
+      </c>
+      <c r="J16" s="17">
+        <f>J13/C13</f>
+        <v>0.14914141414141413</v>
+      </c>
+      <c r="K16" s="17"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="21" spans="1:12" ht="56" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="6">
+        <v>842413</v>
+      </c>
+      <c r="C22" s="6">
+        <v>5842</v>
+      </c>
+      <c r="D22" s="6">
+        <v>36966</v>
+      </c>
+      <c r="E22" s="6">
+        <v>104046</v>
+      </c>
+      <c r="F22" s="6">
+        <v>232969</v>
+      </c>
+      <c r="G22" s="6">
+        <v>2557</v>
+      </c>
+      <c r="H22" s="6">
+        <v>35650</v>
+      </c>
+      <c r="I22" s="7">
+        <v>424383</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <f>C22/B22</f>
+        <v>6.9348407491337388E-3</v>
+      </c>
+      <c r="D23">
+        <f>D22/B22</f>
+        <v>4.3881089204463847E-2</v>
+      </c>
+      <c r="E23">
+        <f>E22/B22</f>
+        <v>0.12350949000074785</v>
+      </c>
+      <c r="F23">
+        <f>F22/B22</f>
+        <v>0.27654962589608661</v>
+      </c>
+      <c r="G23">
+        <f>G22/B22</f>
+        <v>3.0353282772226926E-3</v>
+      </c>
+      <c r="H23">
+        <f>H22/B22</f>
+        <v>4.2318910083296433E-2</v>
+      </c>
+      <c r="I23">
+        <f>I22/B22</f>
+        <v>0.50377071578904886</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="J8:J9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2803CB4-C907-A944-A2A7-4695A544927C}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="56" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="J3" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>0.87</v>
+      </c>
+      <c r="C4">
+        <v>3.27</v>
+      </c>
+      <c r="D4">
+        <v>2.69</v>
+      </c>
+      <c r="E4">
+        <v>22.77</v>
+      </c>
+      <c r="F4">
+        <v>0.3</v>
+      </c>
+      <c r="G4">
+        <v>5.41</v>
+      </c>
+      <c r="H4">
+        <v>64.69</v>
+      </c>
+      <c r="J4" s="21"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J3" r:id="rId1" xr:uid="{1E3840F9-BFE9-EF47-B769-3B28521D9DAC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3679,8 +4448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1A8275-12E4-4647-8849-23CE8825B359}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3785,6 +4554,172 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5136C5-25A9-8446-ABE1-D16B8F03F454}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="B2:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="56" x14ac:dyDescent="0.2">
+      <c r="A1" s="35"/>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="86">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="C2" s="86">
+        <v>4.7100000000000003E-2</v>
+      </c>
+      <c r="D2" s="86">
+        <v>0.12570000000000001</v>
+      </c>
+      <c r="E2" s="86">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="F2" s="86">
+        <v>5.16E-2</v>
+      </c>
+      <c r="G2" s="86">
+        <v>0.55149999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="86">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="C3" s="86">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="D3" s="86">
+        <v>0.1235</v>
+      </c>
+      <c r="E3" s="86">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F3" s="86">
+        <v>4.2299999999999997E-2</v>
+      </c>
+      <c r="G3" s="86">
+        <v>0.50380000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949D2739-F84A-4C43-9937-57F38C57A9F9}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="56" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="66">
+        <v>212000</v>
+      </c>
+      <c r="C2" s="65">
+        <v>674000</v>
+      </c>
+      <c r="D2" s="65">
+        <v>1799000</v>
+      </c>
+      <c r="E2" s="66">
+        <v>42000</v>
+      </c>
+      <c r="F2" s="65">
+        <v>738000</v>
+      </c>
+      <c r="G2" s="65">
+        <v>7895000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="63">
+        <v>5842</v>
+      </c>
+      <c r="C3" s="63">
+        <v>36966</v>
+      </c>
+      <c r="D3" s="63">
+        <v>104046</v>
+      </c>
+      <c r="E3" s="63">
+        <v>2557</v>
+      </c>
+      <c r="F3" s="63">
+        <v>35650</v>
+      </c>
+      <c r="G3" s="64">
+        <v>424383</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E63C8B4A-34CA-D044-894C-1C93961F7DB3}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3823,7 +4758,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92886FB8-A348-9B42-91B6-9401EDCBB5FB}">
   <dimension ref="A1:I14"/>
   <sheetViews>
@@ -4034,7 +4969,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692B5770-BF87-E241-A98B-102B7F0055AF}">
   <dimension ref="A1:M9"/>
   <sheetViews>
@@ -4049,44 +4984,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="71">
+      <c r="B1" s="74">
         <v>2020</v>
       </c>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="69"/>
-      <c r="B2" s="73" t="s">
+      <c r="A2" s="72"/>
+      <c r="B2" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="77" t="s">
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="79" t="s">
+      <c r="J2" s="82" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="102" x14ac:dyDescent="0.2">
-      <c r="A3" s="70"/>
-      <c r="B3" s="74"/>
+      <c r="A3" s="73"/>
+      <c r="B3" s="77"/>
       <c r="C3" s="8" t="s">
         <v>14</v>
       </c>
@@ -4105,8 +5040,8 @@
       <c r="H3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="78"/>
-      <c r="J3" s="80"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="83"/>
       <c r="K3" s="14" t="s">
         <v>23</v>
       </c>
@@ -4289,12 +5224,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A374FE93-5A46-9E4D-82C9-F86D03222DFA}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H5" sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4737,636 +5672,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE57A53-26B7-CD40-AFB1-B8A430F77433}">
-  <dimension ref="A1:M23"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:K13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="56" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2">
-        <v>1.4809640237513098E-2</v>
-      </c>
-      <c r="C2">
-        <v>4.7083478868319942E-2</v>
-      </c>
-      <c r="D2">
-        <v>0.12567237163814182</v>
-      </c>
-      <c r="E2">
-        <v>0.20628711142158576</v>
-      </c>
-      <c r="F2">
-        <v>2.9339853300733498E-3</v>
-      </c>
-      <c r="G2">
-        <v>5.1554313657003144E-2</v>
-      </c>
-      <c r="H2">
-        <v>0.55151938526021704</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3">
-        <v>6.9348407491337388E-3</v>
-      </c>
-      <c r="C3">
-        <v>4.3881089204463847E-2</v>
-      </c>
-      <c r="D3">
-        <v>0.12350949000074785</v>
-      </c>
-      <c r="E3">
-        <v>0.27654962589608661</v>
-      </c>
-      <c r="F3">
-        <v>3.0353282772226926E-3</v>
-      </c>
-      <c r="G3">
-        <v>4.2318910083296433E-2</v>
-      </c>
-      <c r="H3">
-        <v>0.50377071578904886</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="68" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="71">
-        <v>2020</v>
-      </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-    </row>
-    <row r="8" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="69"/>
-      <c r="B8" s="73" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="71" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="76"/>
-      <c r="J8" s="77" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="81" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="102" x14ac:dyDescent="0.2">
-      <c r="A9" s="70"/>
-      <c r="B9" s="74"/>
-      <c r="C9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="78"/>
-      <c r="K9" s="82"/>
-      <c r="L9" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="12">
-        <v>3735</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="13">
-        <v>2597</v>
-      </c>
-      <c r="E10" s="13">
-        <v>591</v>
-      </c>
-      <c r="F10" s="13">
-        <v>70</v>
-      </c>
-      <c r="G10" s="13">
-        <v>217</v>
-      </c>
-      <c r="H10" s="13">
-        <v>14</v>
-      </c>
-      <c r="I10" s="12">
-        <v>246</v>
-      </c>
-      <c r="J10" s="13">
-        <v>970</v>
-      </c>
-      <c r="K10" s="15">
-        <v>1807</v>
-      </c>
-      <c r="L10" s="5">
-        <f>SUM(J10:K10)</f>
-        <v>2777</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="12">
-        <v>3774</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="13">
-        <v>2623</v>
-      </c>
-      <c r="E11" s="13">
-        <v>598</v>
-      </c>
-      <c r="F11" s="13">
-        <v>71</v>
-      </c>
-      <c r="G11" s="13">
-        <v>223</v>
-      </c>
-      <c r="H11" s="13">
-        <v>14</v>
-      </c>
-      <c r="I11" s="12">
-        <v>244</v>
-      </c>
-      <c r="J11" s="13">
-        <v>986</v>
-      </c>
-      <c r="K11" s="15">
-        <v>1819</v>
-      </c>
-      <c r="L11" s="5">
-        <f t="shared" ref="L11:L12" si="0">SUM(J11:K11)</f>
-        <v>2805</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="12">
-        <v>3853</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="13">
-        <v>2675</v>
-      </c>
-      <c r="E12" s="13">
-        <v>610</v>
-      </c>
-      <c r="F12" s="13">
-        <v>71</v>
-      </c>
-      <c r="G12" s="13">
-        <v>234</v>
-      </c>
-      <c r="H12" s="13">
-        <v>14</v>
-      </c>
-      <c r="I12" s="12">
-        <v>248</v>
-      </c>
-      <c r="J12" s="13">
-        <v>997</v>
-      </c>
-      <c r="K12" s="15">
-        <v>1859</v>
-      </c>
-      <c r="L12" s="5">
-        <f t="shared" si="0"/>
-        <v>2856</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="5">
-        <f>SUM(B10:B12)</f>
-        <v>11362</v>
-      </c>
-      <c r="C13" s="5">
-        <v>19800</v>
-      </c>
-      <c r="D13" s="5">
-        <f t="shared" ref="D13:L13" si="1">SUM(D10:D12)</f>
-        <v>7895</v>
-      </c>
-      <c r="E13" s="5">
-        <f t="shared" si="1"/>
-        <v>1799</v>
-      </c>
-      <c r="F13" s="5">
-        <f t="shared" si="1"/>
-        <v>212</v>
-      </c>
-      <c r="G13" s="5">
-        <f t="shared" si="1"/>
-        <v>674</v>
-      </c>
-      <c r="H13" s="5">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-      <c r="I13" s="5">
-        <f t="shared" si="1"/>
-        <v>738</v>
-      </c>
-      <c r="J13" s="5">
-        <f t="shared" si="1"/>
-        <v>2953</v>
-      </c>
-      <c r="K13" s="16">
-        <f t="shared" si="1"/>
-        <v>5485</v>
-      </c>
-      <c r="L13" s="5">
-        <f t="shared" si="1"/>
-        <v>8438</v>
-      </c>
-      <c r="M13" s="5">
-        <f>SUM(B13+L13)</f>
-        <v>19800</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="5">
-        <v>5485</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="5">
-        <v>13380</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17">
-        <v>0.55151938526021704</v>
-      </c>
-      <c r="E16" s="17">
-        <f>E13/C13</f>
-        <v>9.0858585858585861E-2</v>
-      </c>
-      <c r="F16" s="17">
-        <f>F13/C13</f>
-        <v>1.0707070707070707E-2</v>
-      </c>
-      <c r="G16" s="17">
-        <f>G13/C13</f>
-        <v>3.4040404040404038E-2</v>
-      </c>
-      <c r="H16" s="17">
-        <f>H13/C13</f>
-        <v>2.1212121212121214E-3</v>
-      </c>
-      <c r="I16" s="17">
-        <f>I13/C13</f>
-        <v>3.727272727272727E-2</v>
-      </c>
-      <c r="J16" s="17">
-        <f>J13/C13</f>
-        <v>0.14914141414141413</v>
-      </c>
-      <c r="K16" s="17"/>
-      <c r="L16" s="5"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-    </row>
-    <row r="21" spans="1:12" ht="56" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="6">
-        <v>842413</v>
-      </c>
-      <c r="C22" s="6">
-        <v>5842</v>
-      </c>
-      <c r="D22" s="6">
-        <v>36966</v>
-      </c>
-      <c r="E22" s="6">
-        <v>104046</v>
-      </c>
-      <c r="F22" s="6">
-        <v>232969</v>
-      </c>
-      <c r="G22" s="6">
-        <v>2557</v>
-      </c>
-      <c r="H22" s="6">
-        <v>35650</v>
-      </c>
-      <c r="I22" s="7">
-        <v>424383</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C23">
-        <f>C22/B22</f>
-        <v>6.9348407491337388E-3</v>
-      </c>
-      <c r="D23">
-        <f>D22/B22</f>
-        <v>4.3881089204463847E-2</v>
-      </c>
-      <c r="E23">
-        <f>E22/B22</f>
-        <v>0.12350949000074785</v>
-      </c>
-      <c r="F23">
-        <f>F22/B22</f>
-        <v>0.27654962589608661</v>
-      </c>
-      <c r="G23">
-        <f>G22/B22</f>
-        <v>3.0353282772226926E-3</v>
-      </c>
-      <c r="H23">
-        <f>H22/B22</f>
-        <v>4.2318910083296433E-2</v>
-      </c>
-      <c r="I23">
-        <f>I22/B22</f>
-        <v>0.50377071578904886</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="J8:J9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2803CB4-C907-A944-A2A7-4695A544927C}">
-  <dimension ref="A1:J4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="56" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="18"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="J3" s="21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4">
-        <v>0.87</v>
-      </c>
-      <c r="C4">
-        <v>3.27</v>
-      </c>
-      <c r="D4">
-        <v>2.69</v>
-      </c>
-      <c r="E4">
-        <v>22.77</v>
-      </c>
-      <c r="F4">
-        <v>0.3</v>
-      </c>
-      <c r="G4">
-        <v>5.41</v>
-      </c>
-      <c r="H4">
-        <v>64.69</v>
-      </c>
-      <c r="J4" s="21"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="J3" r:id="rId1" xr:uid="{1E3840F9-BFE9-EF47-B769-3B28521D9DAC}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
3_chi_sq_us.qmd --- updated/created kable tables and forrest plots for national odds ratio for dismissal YES
</commit_message>
<xml_diff>
--- a/Data/use_this_replacement_racial_group_representation.xlsx
+++ b/Data/use_this_replacement_racial_group_representation.xlsx
@@ -8,22 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1CBE25-D116-414F-A985-F19D9CF52FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5C96C3-7EC8-0E4C-9B1D-15729E5CE84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="680" windowWidth="19280" windowHeight="14880" firstSheet="3" activeTab="8" xr2:uid="{4D43684D-767A-5B42-8EFD-CDAF7BC426E6}"/>
+    <workbookView xWindow="8500" yWindow="620" windowWidth="19000" windowHeight="15260" firstSheet="6" activeTab="9" xr2:uid="{4D43684D-767A-5B42-8EFD-CDAF7BC426E6}"/>
   </bookViews>
   <sheets>
     <sheet name="2020 national CC vs census" sheetId="4" r:id="rId1"/>
     <sheet name="2020 national CC vs census cha1" sheetId="8" r:id="rId2"/>
     <sheet name="2020 national cc vs census numb" sheetId="10" r:id="rId3"/>
-    <sheet name="2020 national cc vs cen num2 ch" sheetId="12" r:id="rId4"/>
-    <sheet name="2020 national CC vs census num2" sheetId="11" r:id="rId5"/>
-    <sheet name="2020 census vs cc hispanic" sheetId="9" r:id="rId6"/>
-    <sheet name="2020 Child Count" sheetId="1" r:id="rId7"/>
-    <sheet name="2020 Census count" sheetId="2" r:id="rId8"/>
-    <sheet name="2020 census basic table for res" sheetId="6" r:id="rId9"/>
-    <sheet name="2020 % based on census" sheetId="3" r:id="rId10"/>
-    <sheet name="Oregon CC vs census " sheetId="5" r:id="rId11"/>
+    <sheet name="2020 national CC vs census num2" sheetId="11" r:id="rId4"/>
+    <sheet name="2020 national cc vs cen num2 ch" sheetId="12" r:id="rId5"/>
+    <sheet name="2020 Child Count" sheetId="1" r:id="rId6"/>
+    <sheet name="2020 Census count" sheetId="2" r:id="rId7"/>
+    <sheet name="2020 census basic table for res" sheetId="6" r:id="rId8"/>
+    <sheet name="2020 % based on census" sheetId="3" r:id="rId9"/>
+    <sheet name="Oregon CC vs census " sheetId="5" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="59">
   <si>
     <t>State</t>
   </si>
@@ -744,6 +743,7 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="10" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -789,7 +789,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3798,542 +3797,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE57A53-26B7-CD40-AFB1-B8A430F77433}">
-  <dimension ref="A1:M23"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:K13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="56" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2">
-        <v>1.4809640237513098E-2</v>
-      </c>
-      <c r="C2">
-        <v>4.7083478868319942E-2</v>
-      </c>
-      <c r="D2">
-        <v>0.12567237163814182</v>
-      </c>
-      <c r="E2">
-        <v>0.20628711142158576</v>
-      </c>
-      <c r="F2">
-        <v>2.9339853300733498E-3</v>
-      </c>
-      <c r="G2">
-        <v>5.1554313657003144E-2</v>
-      </c>
-      <c r="H2">
-        <v>0.55151938526021704</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3">
-        <v>6.9348407491337388E-3</v>
-      </c>
-      <c r="C3">
-        <v>4.3881089204463847E-2</v>
-      </c>
-      <c r="D3">
-        <v>0.12350949000074785</v>
-      </c>
-      <c r="E3">
-        <v>0.27654962589608661</v>
-      </c>
-      <c r="F3">
-        <v>3.0353282772226926E-3</v>
-      </c>
-      <c r="G3">
-        <v>4.2318910083296433E-2</v>
-      </c>
-      <c r="H3">
-        <v>0.50377071578904886</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="71" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="74">
-        <v>2020</v>
-      </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-    </row>
-    <row r="8" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="72"/>
-      <c r="B8" s="76" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="74" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="79"/>
-      <c r="J8" s="80" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="84" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="102" x14ac:dyDescent="0.2">
-      <c r="A9" s="73"/>
-      <c r="B9" s="77"/>
-      <c r="C9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="81"/>
-      <c r="K9" s="85"/>
-      <c r="L9" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="12">
-        <v>3735</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="13">
-        <v>2597</v>
-      </c>
-      <c r="E10" s="13">
-        <v>591</v>
-      </c>
-      <c r="F10" s="13">
-        <v>70</v>
-      </c>
-      <c r="G10" s="13">
-        <v>217</v>
-      </c>
-      <c r="H10" s="13">
-        <v>14</v>
-      </c>
-      <c r="I10" s="12">
-        <v>246</v>
-      </c>
-      <c r="J10" s="13">
-        <v>970</v>
-      </c>
-      <c r="K10" s="15">
-        <v>1807</v>
-      </c>
-      <c r="L10" s="5">
-        <f>SUM(J10:K10)</f>
-        <v>2777</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="12">
-        <v>3774</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="13">
-        <v>2623</v>
-      </c>
-      <c r="E11" s="13">
-        <v>598</v>
-      </c>
-      <c r="F11" s="13">
-        <v>71</v>
-      </c>
-      <c r="G11" s="13">
-        <v>223</v>
-      </c>
-      <c r="H11" s="13">
-        <v>14</v>
-      </c>
-      <c r="I11" s="12">
-        <v>244</v>
-      </c>
-      <c r="J11" s="13">
-        <v>986</v>
-      </c>
-      <c r="K11" s="15">
-        <v>1819</v>
-      </c>
-      <c r="L11" s="5">
-        <f t="shared" ref="L11:L12" si="0">SUM(J11:K11)</f>
-        <v>2805</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="12">
-        <v>3853</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="13">
-        <v>2675</v>
-      </c>
-      <c r="E12" s="13">
-        <v>610</v>
-      </c>
-      <c r="F12" s="13">
-        <v>71</v>
-      </c>
-      <c r="G12" s="13">
-        <v>234</v>
-      </c>
-      <c r="H12" s="13">
-        <v>14</v>
-      </c>
-      <c r="I12" s="12">
-        <v>248</v>
-      </c>
-      <c r="J12" s="13">
-        <v>997</v>
-      </c>
-      <c r="K12" s="15">
-        <v>1859</v>
-      </c>
-      <c r="L12" s="5">
-        <f t="shared" si="0"/>
-        <v>2856</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="5">
-        <f>SUM(B10:B12)</f>
-        <v>11362</v>
-      </c>
-      <c r="C13" s="5">
-        <v>19800</v>
-      </c>
-      <c r="D13" s="5">
-        <f t="shared" ref="D13:L13" si="1">SUM(D10:D12)</f>
-        <v>7895</v>
-      </c>
-      <c r="E13" s="5">
-        <f t="shared" si="1"/>
-        <v>1799</v>
-      </c>
-      <c r="F13" s="5">
-        <f t="shared" si="1"/>
-        <v>212</v>
-      </c>
-      <c r="G13" s="5">
-        <f t="shared" si="1"/>
-        <v>674</v>
-      </c>
-      <c r="H13" s="5">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-      <c r="I13" s="5">
-        <f t="shared" si="1"/>
-        <v>738</v>
-      </c>
-      <c r="J13" s="5">
-        <f t="shared" si="1"/>
-        <v>2953</v>
-      </c>
-      <c r="K13" s="16">
-        <f t="shared" si="1"/>
-        <v>5485</v>
-      </c>
-      <c r="L13" s="5">
-        <f t="shared" si="1"/>
-        <v>8438</v>
-      </c>
-      <c r="M13" s="5">
-        <f>SUM(B13+L13)</f>
-        <v>19800</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="5">
-        <v>5485</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="5">
-        <v>13380</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17">
-        <v>0.55151938526021704</v>
-      </c>
-      <c r="E16" s="17">
-        <f>E13/C13</f>
-        <v>9.0858585858585861E-2</v>
-      </c>
-      <c r="F16" s="17">
-        <f>F13/C13</f>
-        <v>1.0707070707070707E-2</v>
-      </c>
-      <c r="G16" s="17">
-        <f>G13/C13</f>
-        <v>3.4040404040404038E-2</v>
-      </c>
-      <c r="H16" s="17">
-        <f>H13/C13</f>
-        <v>2.1212121212121214E-3</v>
-      </c>
-      <c r="I16" s="17">
-        <f>I13/C13</f>
-        <v>3.727272727272727E-2</v>
-      </c>
-      <c r="J16" s="17">
-        <f>J13/C13</f>
-        <v>0.14914141414141413</v>
-      </c>
-      <c r="K16" s="17"/>
-      <c r="L16" s="5"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-    </row>
-    <row r="21" spans="1:12" ht="56" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="6">
-        <v>842413</v>
-      </c>
-      <c r="C22" s="6">
-        <v>5842</v>
-      </c>
-      <c r="D22" s="6">
-        <v>36966</v>
-      </c>
-      <c r="E22" s="6">
-        <v>104046</v>
-      </c>
-      <c r="F22" s="6">
-        <v>232969</v>
-      </c>
-      <c r="G22" s="6">
-        <v>2557</v>
-      </c>
-      <c r="H22" s="6">
-        <v>35650</v>
-      </c>
-      <c r="I22" s="7">
-        <v>424383</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C23">
-        <f>C22/B22</f>
-        <v>6.9348407491337388E-3</v>
-      </c>
-      <c r="D23">
-        <f>D22/B22</f>
-        <v>4.3881089204463847E-2</v>
-      </c>
-      <c r="E23">
-        <f>E22/B22</f>
-        <v>0.12350949000074785</v>
-      </c>
-      <c r="F23">
-        <f>F22/B22</f>
-        <v>0.27654962589608661</v>
-      </c>
-      <c r="G23">
-        <f>G22/B22</f>
-        <v>3.0353282772226926E-3</v>
-      </c>
-      <c r="H23">
-        <f>H22/B22</f>
-        <v>4.2318910083296433E-2</v>
-      </c>
-      <c r="I23">
-        <f>I22/B22</f>
-        <v>0.50377071578904886</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="J8:J9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2803CB4-C907-A944-A2A7-4695A544927C}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -4449,7 +3916,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="A1:H3"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4554,93 +4021,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5136C5-25A9-8446-ABE1-D16B8F03F454}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="B2:G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" ht="56" x14ac:dyDescent="0.2">
-      <c r="A1" s="35"/>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="86">
-        <v>1.4800000000000001E-2</v>
-      </c>
-      <c r="C2" s="86">
-        <v>4.7100000000000003E-2</v>
-      </c>
-      <c r="D2" s="86">
-        <v>0.12570000000000001</v>
-      </c>
-      <c r="E2" s="86">
-        <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="F2" s="86">
-        <v>5.16E-2</v>
-      </c>
-      <c r="G2" s="86">
-        <v>0.55149999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="86">
-        <v>6.8999999999999999E-3</v>
-      </c>
-      <c r="C3" s="86">
-        <v>4.3900000000000002E-2</v>
-      </c>
-      <c r="D3" s="86">
-        <v>0.1235</v>
-      </c>
-      <c r="E3" s="86">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F3" s="86">
-        <v>4.2299999999999997E-2</v>
-      </c>
-      <c r="G3" s="86">
-        <v>0.50380000000000003</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949D2739-F84A-4C43-9937-57F38C57A9F9}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4719,51 +4104,54 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E63C8B4A-34CA-D044-894C-1C93961F7DB3}">
-  <dimension ref="A1:B3"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5136C5-25A9-8446-ABE1-D16B8F03F454}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G4" sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="28" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="62" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="65">
-        <v>2953000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="63">
-        <v>232969</v>
-      </c>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="35"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="35"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="35"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92886FB8-A348-9B42-91B6-9401EDCBB5FB}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="I2" sqref="A1:I2"/>
+      <selection activeCell="C14" sqref="A6:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4969,12 +4357,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692B5770-BF87-E241-A98B-102B7F0055AF}">
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J8"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4984,44 +4372,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="74">
+      <c r="B1" s="75">
         <v>2020</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="72"/>
-      <c r="B2" s="76" t="s">
+      <c r="A2" s="73"/>
+      <c r="B2" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="80" t="s">
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="82" t="s">
+      <c r="J2" s="83" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="102" x14ac:dyDescent="0.2">
-      <c r="A3" s="73"/>
-      <c r="B3" s="77"/>
+      <c r="A3" s="74"/>
+      <c r="B3" s="78"/>
       <c r="C3" s="8" t="s">
         <v>14</v>
       </c>
@@ -5040,8 +4428,8 @@
       <c r="H3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="81"/>
-      <c r="J3" s="83"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="84"/>
       <c r="K3" s="14" t="s">
         <v>23</v>
       </c>
@@ -5224,11 +4612,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A374FE93-5A46-9E4D-82C9-F86D03222DFA}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H5" sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
@@ -5672,4 +5060,536 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE57A53-26B7-CD40-AFB1-B8A430F77433}">
+  <dimension ref="A1:M23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="56" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>1.4809640237513098E-2</v>
+      </c>
+      <c r="C2">
+        <v>4.7083478868319942E-2</v>
+      </c>
+      <c r="D2">
+        <v>0.12567237163814182</v>
+      </c>
+      <c r="E2">
+        <v>0.20628711142158576</v>
+      </c>
+      <c r="F2">
+        <v>2.9339853300733498E-3</v>
+      </c>
+      <c r="G2">
+        <v>5.1554313657003144E-2</v>
+      </c>
+      <c r="H2">
+        <v>0.55151938526021704</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>6.9348407491337388E-3</v>
+      </c>
+      <c r="C3">
+        <v>4.3881089204463847E-2</v>
+      </c>
+      <c r="D3">
+        <v>0.12350949000074785</v>
+      </c>
+      <c r="E3">
+        <v>0.27654962589608661</v>
+      </c>
+      <c r="F3">
+        <v>3.0353282772226926E-3</v>
+      </c>
+      <c r="G3">
+        <v>4.2318910083296433E-2</v>
+      </c>
+      <c r="H3">
+        <v>0.50377071578904886</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="75">
+        <v>2020</v>
+      </c>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+    </row>
+    <row r="8" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="73"/>
+      <c r="B8" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="81" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="85" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+      <c r="A9" s="74"/>
+      <c r="B9" s="78"/>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="82"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="12">
+        <v>3735</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="13">
+        <v>2597</v>
+      </c>
+      <c r="E10" s="13">
+        <v>591</v>
+      </c>
+      <c r="F10" s="13">
+        <v>70</v>
+      </c>
+      <c r="G10" s="13">
+        <v>217</v>
+      </c>
+      <c r="H10" s="13">
+        <v>14</v>
+      </c>
+      <c r="I10" s="12">
+        <v>246</v>
+      </c>
+      <c r="J10" s="13">
+        <v>970</v>
+      </c>
+      <c r="K10" s="15">
+        <v>1807</v>
+      </c>
+      <c r="L10" s="5">
+        <f>SUM(J10:K10)</f>
+        <v>2777</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="12">
+        <v>3774</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="13">
+        <v>2623</v>
+      </c>
+      <c r="E11" s="13">
+        <v>598</v>
+      </c>
+      <c r="F11" s="13">
+        <v>71</v>
+      </c>
+      <c r="G11" s="13">
+        <v>223</v>
+      </c>
+      <c r="H11" s="13">
+        <v>14</v>
+      </c>
+      <c r="I11" s="12">
+        <v>244</v>
+      </c>
+      <c r="J11" s="13">
+        <v>986</v>
+      </c>
+      <c r="K11" s="15">
+        <v>1819</v>
+      </c>
+      <c r="L11" s="5">
+        <f t="shared" ref="L11:L12" si="0">SUM(J11:K11)</f>
+        <v>2805</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="12">
+        <v>3853</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="13">
+        <v>2675</v>
+      </c>
+      <c r="E12" s="13">
+        <v>610</v>
+      </c>
+      <c r="F12" s="13">
+        <v>71</v>
+      </c>
+      <c r="G12" s="13">
+        <v>234</v>
+      </c>
+      <c r="H12" s="13">
+        <v>14</v>
+      </c>
+      <c r="I12" s="12">
+        <v>248</v>
+      </c>
+      <c r="J12" s="13">
+        <v>997</v>
+      </c>
+      <c r="K12" s="15">
+        <v>1859</v>
+      </c>
+      <c r="L12" s="5">
+        <f t="shared" si="0"/>
+        <v>2856</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B13" s="5">
+        <f>SUM(B10:B12)</f>
+        <v>11362</v>
+      </c>
+      <c r="C13" s="5">
+        <v>19800</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" ref="D13:L13" si="1">SUM(D10:D12)</f>
+        <v>7895</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>1799</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="1"/>
+        <v>212</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="1"/>
+        <v>674</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" si="1"/>
+        <v>738</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" si="1"/>
+        <v>2953</v>
+      </c>
+      <c r="K13" s="16">
+        <f t="shared" si="1"/>
+        <v>5485</v>
+      </c>
+      <c r="L13" s="5">
+        <f t="shared" si="1"/>
+        <v>8438</v>
+      </c>
+      <c r="M13" s="5">
+        <f>SUM(B13+L13)</f>
+        <v>19800</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="5">
+        <v>5485</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="5">
+        <v>13380</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17">
+        <v>0.55151938526021704</v>
+      </c>
+      <c r="E16" s="17">
+        <f>E13/C13</f>
+        <v>9.0858585858585861E-2</v>
+      </c>
+      <c r="F16" s="17">
+        <f>F13/C13</f>
+        <v>1.0707070707070707E-2</v>
+      </c>
+      <c r="G16" s="17">
+        <f>G13/C13</f>
+        <v>3.4040404040404038E-2</v>
+      </c>
+      <c r="H16" s="17">
+        <f>H13/C13</f>
+        <v>2.1212121212121214E-3</v>
+      </c>
+      <c r="I16" s="17">
+        <f>I13/C13</f>
+        <v>3.727272727272727E-2</v>
+      </c>
+      <c r="J16" s="17">
+        <f>J13/C13</f>
+        <v>0.14914141414141413</v>
+      </c>
+      <c r="K16" s="17"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="21" spans="1:12" ht="56" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="6">
+        <v>842413</v>
+      </c>
+      <c r="C22" s="6">
+        <v>5842</v>
+      </c>
+      <c r="D22" s="6">
+        <v>36966</v>
+      </c>
+      <c r="E22" s="6">
+        <v>104046</v>
+      </c>
+      <c r="F22" s="6">
+        <v>232969</v>
+      </c>
+      <c r="G22" s="6">
+        <v>2557</v>
+      </c>
+      <c r="H22" s="6">
+        <v>35650</v>
+      </c>
+      <c r="I22" s="7">
+        <v>424383</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <f>C22/B22</f>
+        <v>6.9348407491337388E-3</v>
+      </c>
+      <c r="D23">
+        <f>D22/B22</f>
+        <v>4.3881089204463847E-2</v>
+      </c>
+      <c r="E23">
+        <f>E22/B22</f>
+        <v>0.12350949000074785</v>
+      </c>
+      <c r="F23">
+        <f>F22/B22</f>
+        <v>0.27654962589608661</v>
+      </c>
+      <c r="G23">
+        <f>G22/B22</f>
+        <v>3.0353282772226926E-3</v>
+      </c>
+      <c r="H23">
+        <f>H22/B22</f>
+        <v>4.2318910083296433E-2</v>
+      </c>
+      <c r="I23">
+        <f>I22/B22</f>
+        <v>0.50377071578904886</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="J8:J9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
3_chi_sq_us.qmd --- updated the tables and plots with standardized residuals for national exit patterns by race. Beauty :)
</commit_message>
<xml_diff>
--- a/Data/use_this_replacement_racial_group_representation.xlsx
+++ b/Data/use_this_replacement_racial_group_representation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5C96C3-7EC8-0E4C-9B1D-15729E5CE84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A2106D-A0AE-2343-B978-7C71C614346B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8500" yWindow="620" windowWidth="19000" windowHeight="15260" firstSheet="6" activeTab="9" xr2:uid="{4D43684D-767A-5B42-8EFD-CDAF7BC426E6}"/>
+    <workbookView xWindow="1780" yWindow="860" windowWidth="25220" windowHeight="15540" firstSheet="3" activeTab="4" xr2:uid="{4D43684D-767A-5B42-8EFD-CDAF7BC426E6}"/>
   </bookViews>
   <sheets>
     <sheet name="2020 national CC vs census" sheetId="4" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="63">
   <si>
     <t>State</t>
   </si>
@@ -257,6 +257,18 @@
   <si>
     <t>Total - Hispanic</t>
   </si>
+  <si>
+    <t xml:space="preserve">White </t>
+  </si>
+  <si>
+    <t>General Populatiom %</t>
+  </si>
+  <si>
+    <t>THIS INCLUDES HISPANIC AS a part of the race, so below I TOOK OUT Hispanic entirely from EI and did the ratio</t>
+  </si>
+  <si>
+    <t>EI %</t>
+  </si>
 </sst>
 </file>
 
@@ -265,7 +277,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -350,6 +362,30 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -575,7 +611,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -789,6 +825,29 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1459,6 +1518,798 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2020 national cc vs cen num2 ch'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>General Population </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="88500"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2020 national cc vs cen num2 ch'!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>American Indian or Alaska Native</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Asian</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Black or African American</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Hispanic/Latino</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Native Hawaiian or Pacific Islander</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Two or More Races</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>White </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2020 national cc vs cen num2 ch'!$B$2:$H$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.8661971830985915E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9330985915492955E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15836267605633803</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6971830985915491E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.4964788732394363E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.69498239436619713</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-343B-A645-B71E-8BF8BC933A3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2020 national cc vs cen num2 ch'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EI Population </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="55000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2020 national cc vs cen num2 ch'!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>American Indian or Alaska Native</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Asian</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Black or African American</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Hispanic/Latino</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Native Hawaiian or Pacific Islander</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Two or More Races</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>White </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2020 national cc vs cen num2 ch'!$B$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.8999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3900000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1235</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7650000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.2299999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.50380000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-343B-A645-B71E-8BF8BC933A3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="784441407"/>
+        <c:axId val="819417263"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="784441407"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="819417263"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="819417263"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="784441407"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1000" baseline="0">
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2020 national cc vs cen num2 ch'!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>General Population </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="88500"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2020 national cc vs cen num2 ch'!$B$26:$G$26</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>American Indian or Alaska Native</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Asian</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Black or African American</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Native Hawaiian or Pacific Islander</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Two or More Races</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>White </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2020 national cc vs cen num2 ch'!$B$27:$G$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.8661971830985915E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9330985915492955E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15836267605633803</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6971830985915491E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4964788732394363E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.69498239436619713</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D9DB-744A-9364-7925CD98EF5E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2020 national cc vs cen num2 ch'!$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EI Population </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="55000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2020 national cc vs cen num2 ch'!$B$26:$G$26</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>American Indian or Alaska Native</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Asian</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Black or African American</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Native Hawaiian or Pacific Islander</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Two or More Races</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>White </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2020 national cc vs cen num2 ch'!$B$28:$G$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.5999999999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0699999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17069999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1999999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8500000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.69630000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D9DB-744A-9364-7925CD98EF5E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="736165760"/>
+        <c:axId val="736189696"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="736165760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="736189696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="736189696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="736165760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1988,6 +2839,60 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
+  <cs:variation>
+    <a:tint val="88500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="55000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="75000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="98500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="80000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
+  <cs:variation>
+    <a:tint val="88500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="55000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="75000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="98500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="80000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2533,6 +3438,1012 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3082,6 +4993,83 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27F97343-0668-8E50-8CD5-FAFC2003913E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47B89F7A-E89B-0864-D2FB-C62BCF4CAD6D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
@@ -3129,7 +5117,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3178,7 +5166,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3800,7 +5788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2803CB4-C907-A944-A2A7-4695A544927C}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -4025,7 +6013,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G3" sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4106,43 +6094,475 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5136C5-25A9-8446-ABE1-D16B8F03F454}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="A1:G4"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G28" sqref="A26:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="68.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="35"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="35"/>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="35"/>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
+    <row r="1" spans="1:9" ht="56" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="22">
+        <v>1.8661971830985915E-2</v>
+      </c>
+      <c r="C2" s="22">
+        <v>5.9330985915492955E-2</v>
+      </c>
+      <c r="D2" s="22">
+        <v>0.15836267605633803</v>
+      </c>
+      <c r="F2" s="22">
+        <v>3.6971830985915491E-3</v>
+      </c>
+      <c r="G2" s="22">
+        <v>6.4964788732394363E-2</v>
+      </c>
+      <c r="H2" s="22">
+        <v>0.69498239436619713</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="87">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="C3" s="88">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="D3" s="88">
+        <v>0.1235</v>
+      </c>
+      <c r="E3" s="88">
+        <v>2.7650000000000001E-2</v>
+      </c>
+      <c r="F3" s="88">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G3" s="88">
+        <v>4.2299999999999997E-2</v>
+      </c>
+      <c r="H3" s="88">
+        <v>0.50380000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+    </row>
+    <row r="8" spans="1:9" ht="56" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="66">
+        <v>212000</v>
+      </c>
+      <c r="C9" s="65">
+        <v>674000</v>
+      </c>
+      <c r="D9" s="65">
+        <v>1799000</v>
+      </c>
+      <c r="E9" s="66">
+        <v>42000</v>
+      </c>
+      <c r="F9" s="65">
+        <v>738000</v>
+      </c>
+      <c r="G9" s="65">
+        <v>7895000</v>
+      </c>
+      <c r="H9" s="67">
+        <v>11360000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="63">
+        <v>5842</v>
+      </c>
+      <c r="C10" s="63">
+        <v>36966</v>
+      </c>
+      <c r="D10" s="63">
+        <v>104046</v>
+      </c>
+      <c r="E10" s="63">
+        <v>2557</v>
+      </c>
+      <c r="F10" s="63">
+        <v>35650</v>
+      </c>
+      <c r="G10" s="64">
+        <v>424383</v>
+      </c>
+      <c r="I10" s="89" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I11" s="89"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <f>B9/H9</f>
+        <v>1.8661971830985915E-2</v>
+      </c>
+      <c r="C12">
+        <f>C9/H9</f>
+        <v>5.9330985915492955E-2</v>
+      </c>
+      <c r="D12">
+        <f>D9/H9</f>
+        <v>0.15836267605633803</v>
+      </c>
+      <c r="E12">
+        <f>E9/H9</f>
+        <v>3.6971830985915491E-3</v>
+      </c>
+      <c r="F12">
+        <f>F9/H9</f>
+        <v>6.4964788732394363E-2</v>
+      </c>
+      <c r="G12">
+        <f>G9/H9</f>
+        <v>0.69498239436619713</v>
+      </c>
+      <c r="H12">
+        <f>SUM(B12:G12)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="I12" s="89"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="22">
+        <v>1.8661971830985915E-2</v>
+      </c>
+      <c r="C13" s="22">
+        <v>5.9330985915492955E-2</v>
+      </c>
+      <c r="D13" s="22">
+        <v>0.15836267605633803</v>
+      </c>
+      <c r="E13" s="22">
+        <v>3.6971830985915491E-3</v>
+      </c>
+      <c r="F13" s="22">
+        <v>6.4964788732394363E-2</v>
+      </c>
+      <c r="G13" s="22">
+        <v>0.69498239436619713</v>
+      </c>
+      <c r="H13" s="22">
+        <f>SUM(B13:G13)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="I13" s="89"/>
+    </row>
+    <row r="16" spans="1:9" ht="56" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="66">
+        <v>212000</v>
+      </c>
+      <c r="C17" s="65">
+        <v>674000</v>
+      </c>
+      <c r="D17" s="65">
+        <v>1799000</v>
+      </c>
+      <c r="E17" s="66">
+        <v>42000</v>
+      </c>
+      <c r="F17" s="65">
+        <v>738000</v>
+      </c>
+      <c r="G17" s="65">
+        <v>7895000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="63">
+        <v>5842</v>
+      </c>
+      <c r="C18" s="63">
+        <v>36966</v>
+      </c>
+      <c r="D18" s="63">
+        <v>104046</v>
+      </c>
+      <c r="E18" s="63">
+        <v>2557</v>
+      </c>
+      <c r="F18" s="63">
+        <v>35650</v>
+      </c>
+      <c r="G18" s="64">
+        <v>424383</v>
+      </c>
+      <c r="H18" s="5">
+        <f>SUM(B18:G18)</f>
+        <v>609444</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="22">
+        <f>B18/H18</f>
+        <v>9.5857863889052975E-3</v>
+      </c>
+      <c r="C20" s="22">
+        <f>C18/H18</f>
+        <v>6.0655285801484632E-2</v>
+      </c>
+      <c r="D20" s="22">
+        <f>D18/H18</f>
+        <v>0.1707228227696064</v>
+      </c>
+      <c r="E20" s="22">
+        <f>E18/H18</f>
+        <v>4.1956274899744685E-3</v>
+      </c>
+      <c r="F20" s="22">
+        <f>F18/H18</f>
+        <v>5.8495940562217366E-2</v>
+      </c>
+      <c r="G20" s="22">
+        <f>G18/H18</f>
+        <v>0.69634453698781185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="56" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="22">
+        <v>1.8661971830985915E-2</v>
+      </c>
+      <c r="C23" s="22">
+        <v>5.9330985915492955E-2</v>
+      </c>
+      <c r="D23" s="22">
+        <v>0.15836267605633803</v>
+      </c>
+      <c r="E23" s="22">
+        <v>3.6971830985915491E-3</v>
+      </c>
+      <c r="F23" s="22">
+        <v>6.4964788732394363E-2</v>
+      </c>
+      <c r="G23" s="22">
+        <v>0.69498239436619713</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="87">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="C24" s="88">
+        <v>6.0699999999999997E-2</v>
+      </c>
+      <c r="D24" s="88">
+        <v>0.17069999999999999</v>
+      </c>
+      <c r="E24" s="88">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="F24" s="88">
+        <v>5.8500000000000003E-2</v>
+      </c>
+      <c r="G24" s="88">
+        <v>0.69630000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.2">
+      <c r="A26" s="96"/>
+      <c r="B26" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="92" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="91" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="92" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="92" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="90" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="93">
+        <v>1.8661971830985915E-2</v>
+      </c>
+      <c r="C27" s="93">
+        <v>5.9330985915492955E-2</v>
+      </c>
+      <c r="D27" s="93">
+        <v>0.15836267605633803</v>
+      </c>
+      <c r="E27" s="93">
+        <v>3.6971830985915491E-3</v>
+      </c>
+      <c r="F27" s="93">
+        <v>6.4964788732394363E-2</v>
+      </c>
+      <c r="G27" s="93">
+        <v>0.69498239436619713</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="94">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="C28" s="95">
+        <v>6.0699999999999997E-2</v>
+      </c>
+      <c r="D28" s="95">
+        <v>0.17069999999999999</v>
+      </c>
+      <c r="E28" s="95">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="F28" s="95">
+        <v>5.8500000000000003E-2</v>
+      </c>
+      <c r="G28" s="95">
+        <v>0.69630000000000003</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I10:I13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Final backup from my work laptop before maintenance
</commit_message>
<xml_diff>
--- a/Data/use_this_replacement_racial_group_representation.xlsx
+++ b/Data/use_this_replacement_racial_group_representation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A2106D-A0AE-2343-B978-7C71C614346B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821CAF9D-3956-8744-BB22-B75109ABCC89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="860" windowWidth="25220" windowHeight="15540" firstSheet="3" activeTab="4" xr2:uid="{4D43684D-767A-5B42-8EFD-CDAF7BC426E6}"/>
+    <workbookView xWindow="3380" yWindow="860" windowWidth="25220" windowHeight="15540" firstSheet="3" activeTab="4" xr2:uid="{4D43684D-767A-5B42-8EFD-CDAF7BC426E6}"/>
   </bookViews>
   <sheets>
     <sheet name="2020 national CC vs census" sheetId="4" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="63">
   <si>
     <t>State</t>
   </si>
@@ -611,7 +611,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -780,6 +780,29 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -825,29 +848,30 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6094,10 +6118,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5136C5-25A9-8446-ABE1-D16B8F03F454}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G28" sqref="A26:G28"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6155,25 +6179,25 @@
       <c r="A3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="87">
+      <c r="B3" s="72">
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="C3" s="88">
+      <c r="C3" s="73">
         <v>4.3900000000000002E-2</v>
       </c>
-      <c r="D3" s="88">
+      <c r="D3" s="73">
         <v>0.1235</v>
       </c>
-      <c r="E3" s="88">
+      <c r="E3" s="73">
         <v>2.7650000000000001E-2</v>
       </c>
-      <c r="F3" s="88">
+      <c r="F3" s="73">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="G3" s="88">
+      <c r="G3" s="73">
         <v>4.2299999999999997E-2</v>
       </c>
-      <c r="H3" s="88">
+      <c r="H3" s="73">
         <v>0.50380000000000003</v>
       </c>
     </row>
@@ -6255,12 +6279,12 @@
       <c r="G10" s="64">
         <v>424383</v>
       </c>
-      <c r="I10" s="89" t="s">
+      <c r="I10" s="82" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I11" s="89"/>
+      <c r="I11" s="82"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -6294,7 +6318,7 @@
         <f>SUM(B12:G12)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="I12" s="89"/>
+      <c r="I12" s="82"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="22">
@@ -6319,7 +6343,7 @@
         <f>SUM(B13:G13)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="I13" s="89"/>
+      <c r="I13" s="82"/>
     </row>
     <row r="16" spans="1:9" ht="56" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -6470,89 +6494,164 @@
       <c r="A24" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="87">
+      <c r="B24" s="72">
         <v>9.5999999999999992E-3</v>
       </c>
-      <c r="C24" s="88">
+      <c r="C24" s="73">
         <v>6.0699999999999997E-2</v>
       </c>
-      <c r="D24" s="88">
+      <c r="D24" s="73">
         <v>0.17069999999999999</v>
       </c>
-      <c r="E24" s="88">
+      <c r="E24" s="73">
         <v>4.1999999999999997E-3</v>
       </c>
-      <c r="F24" s="88">
+      <c r="F24" s="73">
         <v>5.8500000000000003E-2</v>
       </c>
-      <c r="G24" s="88">
+      <c r="G24" s="73">
         <v>0.69630000000000003</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.2">
-      <c r="A26" s="96"/>
-      <c r="B26" s="91" t="s">
+      <c r="A26" s="80"/>
+      <c r="B26" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="92" t="s">
+      <c r="C26" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="92" t="s">
+      <c r="D26" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="91" t="s">
+      <c r="E26" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="92" t="s">
+      <c r="F26" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="92" t="s">
+      <c r="G26" s="76" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="90" t="s">
+      <c r="A27" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="93">
+      <c r="B27" s="77">
         <v>1.8661971830985915E-2</v>
       </c>
-      <c r="C27" s="93">
+      <c r="C27" s="77">
         <v>5.9330985915492955E-2</v>
       </c>
-      <c r="D27" s="93">
+      <c r="D27" s="77">
         <v>0.15836267605633803</v>
       </c>
-      <c r="E27" s="93">
+      <c r="E27" s="77">
         <v>3.6971830985915491E-3</v>
       </c>
-      <c r="F27" s="93">
+      <c r="F27" s="77">
         <v>6.4964788732394363E-2</v>
       </c>
-      <c r="G27" s="93">
+      <c r="G27" s="77">
         <v>0.69498239436619713</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="97" t="s">
+      <c r="A28" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="94">
+      <c r="B28" s="78">
         <v>9.5999999999999992E-3</v>
       </c>
-      <c r="C28" s="95">
+      <c r="C28" s="79">
         <v>6.0699999999999997E-2</v>
       </c>
-      <c r="D28" s="95">
+      <c r="D28" s="79">
         <v>0.17069999999999999</v>
       </c>
-      <c r="E28" s="95">
+      <c r="E28" s="79">
         <v>4.1999999999999997E-3</v>
       </c>
-      <c r="F28" s="95">
+      <c r="F28" s="79">
         <v>5.8500000000000003E-2</v>
       </c>
-      <c r="G28" s="95">
+      <c r="G28" s="79">
+        <v>0.69630000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="98"/>
+      <c r="B31" s="99" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="100" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.2">
+      <c r="A32" s="101" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="102">
+        <v>1.8661971830985915E-2</v>
+      </c>
+      <c r="C32" s="103">
+        <v>9.5999999999999992E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="104" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="102">
+        <v>5.9330985915492955E-2</v>
+      </c>
+      <c r="C33" s="105">
+        <v>6.0699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="A34" s="104" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="102">
+        <v>0.15836267605633803</v>
+      </c>
+      <c r="C34" s="105">
+        <v>0.17069999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+      <c r="A35" s="101" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="102">
+        <v>3.6971830985915491E-3</v>
+      </c>
+      <c r="C35" s="105">
+        <v>4.1999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A36" s="104" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="102">
+        <v>6.4964788732394363E-2</v>
+      </c>
+      <c r="C36" s="105">
+        <v>5.8500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="104" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="102">
+        <v>0.69498239436619713</v>
+      </c>
+      <c r="C37" s="105">
         <v>0.69630000000000003</v>
       </c>
     </row>
@@ -6792,44 +6891,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="75">
+      <c r="B1" s="86">
         <v>2020</v>
       </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="73"/>
-      <c r="B2" s="77" t="s">
+      <c r="A2" s="84"/>
+      <c r="B2" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="81" t="s">
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="83" t="s">
+      <c r="J2" s="94" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="102" x14ac:dyDescent="0.2">
-      <c r="A3" s="74"/>
-      <c r="B3" s="78"/>
+      <c r="A3" s="85"/>
+      <c r="B3" s="89"/>
       <c r="C3" s="8" t="s">
         <v>14</v>
       </c>
@@ -6848,8 +6947,8 @@
       <c r="H3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="82"/>
-      <c r="J3" s="84"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="95"/>
       <c r="K3" s="14" t="s">
         <v>23</v>
       </c>
@@ -7572,44 +7671,44 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="75">
+      <c r="B7" s="86">
         <v>2020</v>
       </c>
-      <c r="C7" s="76"/>
-      <c r="D7" s="76"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="87"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
     </row>
     <row r="8" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="73"/>
-      <c r="B8" s="77" t="s">
+      <c r="A8" s="84"/>
+      <c r="B8" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="75" t="s">
+      <c r="D8" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="79"/>
-      <c r="I8" s="80"/>
-      <c r="J8" s="81" t="s">
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="91"/>
+      <c r="J8" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="85" t="s">
+      <c r="K8" s="96" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="102" x14ac:dyDescent="0.2">
-      <c r="A9" s="74"/>
-      <c r="B9" s="78"/>
+      <c r="A9" s="85"/>
+      <c r="B9" s="89"/>
       <c r="C9" t="s">
         <v>36</v>
       </c>
@@ -7631,8 +7730,8 @@
       <c r="I9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="82"/>
-      <c r="K9" s="86"/>
+      <c r="J9" s="93"/>
+      <c r="K9" s="97"/>
       <c r="L9" s="14" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
1_clean_data.qmd --- updated Kable tables to include ratio
</commit_message>
<xml_diff>
--- a/Data/use_this_replacement_racial_group_representation.xlsx
+++ b/Data/use_this_replacement_racial_group_representation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821CAF9D-3956-8744-BB22-B75109ABCC89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD87A44D-53A2-B248-BFD6-3801B8069BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="860" windowWidth="25220" windowHeight="15540" firstSheet="3" activeTab="4" xr2:uid="{4D43684D-767A-5B42-8EFD-CDAF7BC426E6}"/>
+    <workbookView xWindow="3380" yWindow="820" windowWidth="25220" windowHeight="15540" firstSheet="4" activeTab="6" xr2:uid="{4D43684D-767A-5B42-8EFD-CDAF7BC426E6}"/>
   </bookViews>
   <sheets>
     <sheet name="2020 national CC vs census" sheetId="4" r:id="rId1"/>
@@ -802,6 +802,30 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -847,30 +871,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6120,7 +6120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5136C5-25A9-8446-ABE1-D16B8F03F454}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="F26" workbookViewId="0">
       <selection activeCell="A31" sqref="A31:C37"/>
     </sheetView>
   </sheetViews>
@@ -6279,12 +6279,12 @@
       <c r="G10" s="64">
         <v>424383</v>
       </c>
-      <c r="I10" s="82" t="s">
+      <c r="I10" s="90" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I11" s="82"/>
+      <c r="I11" s="90"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -6318,7 +6318,7 @@
         <f>SUM(B12:G12)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="I12" s="82"/>
+      <c r="I12" s="90"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="22">
@@ -6343,7 +6343,7 @@
         <f>SUM(B13:G13)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="I13" s="82"/>
+      <c r="I13" s="90"/>
     </row>
     <row r="16" spans="1:9" ht="56" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -6581,77 +6581,77 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="98"/>
-      <c r="B31" s="99" t="s">
+      <c r="A31" s="82"/>
+      <c r="B31" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="100" t="s">
+      <c r="C31" s="84" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.2">
-      <c r="A32" s="101" t="s">
+      <c r="A32" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="102">
+      <c r="B32" s="86">
         <v>1.8661971830985915E-2</v>
       </c>
-      <c r="C32" s="103">
+      <c r="C32" s="87">
         <v>9.5999999999999992E-3</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="104" t="s">
+      <c r="A33" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="102">
+      <c r="B33" s="86">
         <v>5.9330985915492955E-2</v>
       </c>
-      <c r="C33" s="105">
+      <c r="C33" s="89">
         <v>6.0699999999999997E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A34" s="104" t="s">
+      <c r="A34" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="102">
+      <c r="B34" s="86">
         <v>0.15836267605633803</v>
       </c>
-      <c r="C34" s="105">
+      <c r="C34" s="89">
         <v>0.17069999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="60" x14ac:dyDescent="0.2">
-      <c r="A35" s="101" t="s">
+      <c r="A35" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="102">
+      <c r="B35" s="86">
         <v>3.6971830985915491E-3</v>
       </c>
-      <c r="C35" s="105">
+      <c r="C35" s="89">
         <v>4.1999999999999997E-3</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A36" s="104" t="s">
+      <c r="A36" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="102">
+      <c r="B36" s="86">
         <v>6.4964788732394363E-2</v>
       </c>
-      <c r="C36" s="105">
+      <c r="C36" s="89">
         <v>5.8500000000000003E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="104" t="s">
+      <c r="A37" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="102">
+      <c r="B37" s="86">
         <v>0.69498239436619713</v>
       </c>
-      <c r="C37" s="105">
+      <c r="C37" s="89">
         <v>0.69630000000000003</v>
       </c>
     </row>
@@ -6880,7 +6880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692B5770-BF87-E241-A98B-102B7F0055AF}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -6891,44 +6891,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="86">
+      <c r="B1" s="94">
         <v>2020</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="84"/>
-      <c r="B2" s="88" t="s">
+      <c r="A2" s="92"/>
+      <c r="B2" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="92" t="s">
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="94" t="s">
+      <c r="J2" s="102" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="102" x14ac:dyDescent="0.2">
-      <c r="A3" s="85"/>
-      <c r="B3" s="89"/>
+      <c r="A3" s="93"/>
+      <c r="B3" s="97"/>
       <c r="C3" s="8" t="s">
         <v>14</v>
       </c>
@@ -6947,8 +6947,8 @@
       <c r="H3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="93"/>
-      <c r="J3" s="95"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="103"/>
       <c r="K3" s="14" t="s">
         <v>23</v>
       </c>
@@ -7671,44 +7671,44 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="86">
+      <c r="B7" s="94">
         <v>2020</v>
       </c>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="87"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="95"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="95"/>
     </row>
     <row r="8" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="84"/>
-      <c r="B8" s="88" t="s">
+      <c r="A8" s="92"/>
+      <c r="B8" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="86" t="s">
+      <c r="D8" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="90"/>
-      <c r="H8" s="90"/>
-      <c r="I8" s="91"/>
-      <c r="J8" s="92" t="s">
+      <c r="E8" s="98"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98"/>
+      <c r="H8" s="98"/>
+      <c r="I8" s="99"/>
+      <c r="J8" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="96" t="s">
+      <c r="K8" s="104" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="102" x14ac:dyDescent="0.2">
-      <c r="A9" s="85"/>
-      <c r="B9" s="89"/>
+      <c r="A9" s="93"/>
+      <c r="B9" s="97"/>
       <c r="C9" t="s">
         <v>36</v>
       </c>
@@ -7730,8 +7730,8 @@
       <c r="I9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="93"/>
-      <c r="K9" s="97"/>
+      <c r="J9" s="101"/>
+      <c r="K9" s="105"/>
       <c r="L9" s="14" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
race_oregon_chart df and csv --- cleaned up for dissertation results table
</commit_message>
<xml_diff>
--- a/Data/use_this_replacement_racial_group_representation.xlsx
+++ b/Data/use_this_replacement_racial_group_representation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD87A44D-53A2-B248-BFD6-3801B8069BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BA05EE-9536-F340-B9D5-F1C78BE4A1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="820" windowWidth="25220" windowHeight="15540" firstSheet="4" activeTab="6" xr2:uid="{4D43684D-767A-5B42-8EFD-CDAF7BC426E6}"/>
+    <workbookView xWindow="4560" yWindow="540" windowWidth="25220" windowHeight="15540" firstSheet="4" activeTab="4" xr2:uid="{4D43684D-767A-5B42-8EFD-CDAF7BC426E6}"/>
   </bookViews>
   <sheets>
     <sheet name="2020 national CC vs census" sheetId="4" r:id="rId1"/>
@@ -1567,406 +1567,6 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2020 national cc vs cen num2 ch'!$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>General Population </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:tint val="88500"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'2020 national cc vs cen num2 ch'!$B$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>American Indian or Alaska Native</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Asian</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Black or African American</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Hispanic/Latino</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Native Hawaiian or Pacific Islander</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Two or More Races</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>White </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2020 national cc vs cen num2 ch'!$B$2:$H$2</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.8661971830985915E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.9330985915492955E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.15836267605633803</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.6971830985915491E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.4964788732394363E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.69498239436619713</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-343B-A645-B71E-8BF8BC933A3E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2020 national cc vs cen num2 ch'!$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>EI Population </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:tint val="55000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'2020 national cc vs cen num2 ch'!$B$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>American Indian or Alaska Native</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Asian</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Black or African American</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Hispanic/Latino</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Native Hawaiian or Pacific Islander</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Two or More Races</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>White </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2020 national cc vs cen num2 ch'!$B$3:$H$3</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>6.8999999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.3900000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.1235</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.7650000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.2299999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.50380000000000003</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-343B-A645-B71E-8BF8BC933A3E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="784441407"/>
-        <c:axId val="819417263"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="784441407"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="819417263"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="819417263"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="784441407"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1000" baseline="0">
-          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="1"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
               <c:f>'2020 national cc vs cen num2 ch'!$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -2333,7 +1933,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2890,33 +2490,6 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
-  <a:schemeClr val="dk1"/>
-  <cs:variation>
-    <a:tint val="88500"/>
-  </cs:variation>
-  <cs:variation>
-    <a:tint val="55000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:tint val="75000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:tint val="98500"/>
-  </cs:variation>
-  <cs:variation>
-    <a:tint val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:tint val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:tint val="80000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3965,509 +3538,6 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5019,42 +4089,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27F97343-0668-8E50-8CD5-FAFC2003913E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>107950</xdr:colOff>
       <xdr:row>14</xdr:row>
@@ -5083,7 +4117,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6120,8 +5154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5136C5-25A9-8446-ABE1-D16B8F03F454}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView topLeftCell="F26" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:C37"/>
+    <sheetView tabSelected="1" topLeftCell="F16" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6880,7 +5914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692B5770-BF87-E241-A98B-102B7F0055AF}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
data folder update --- I added a sheet/chart to use_this_replacement_racial_group_representation.xlsx
</commit_message>
<xml_diff>
--- a/Data/use_this_replacement_racial_group_representation.xlsx
+++ b/Data/use_this_replacement_racial_group_representation.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BA05EE-9536-F340-B9D5-F1C78BE4A1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5612FFF7-523F-8D4F-A608-6ADF2E6F0F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="540" windowWidth="25220" windowHeight="15540" firstSheet="4" activeTab="4" xr2:uid="{4D43684D-767A-5B42-8EFD-CDAF7BC426E6}"/>
+    <workbookView xWindow="12460" yWindow="720" windowWidth="25100" windowHeight="15540" firstSheet="1" activeTab="2" xr2:uid="{4D43684D-767A-5B42-8EFD-CDAF7BC426E6}"/>
   </bookViews>
   <sheets>
     <sheet name="2020 national CC vs census" sheetId="4" r:id="rId1"/>
-    <sheet name="2020 national CC vs census cha1" sheetId="8" r:id="rId2"/>
-    <sheet name="2020 national cc vs census numb" sheetId="10" r:id="rId3"/>
-    <sheet name="2020 national CC vs census num2" sheetId="11" r:id="rId4"/>
-    <sheet name="2020 national cc vs cen num2 ch" sheetId="12" r:id="rId5"/>
-    <sheet name="2020 Child Count" sheetId="1" r:id="rId6"/>
-    <sheet name="2020 Census count" sheetId="2" r:id="rId7"/>
-    <sheet name="2020 census basic table for res" sheetId="6" r:id="rId8"/>
-    <sheet name="2020 % based on census" sheetId="3" r:id="rId9"/>
-    <sheet name="Oregon CC vs census " sheetId="5" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId2"/>
+    <sheet name="2020 Oregon child count" sheetId="14" r:id="rId3"/>
+    <sheet name="2020 national CC vs census cha1" sheetId="8" r:id="rId4"/>
+    <sheet name="2020 national cc vs census numb" sheetId="10" r:id="rId5"/>
+    <sheet name="2020 national CC vs census num2" sheetId="11" r:id="rId6"/>
+    <sheet name="2020 national cc vs cen num2 ch" sheetId="12" r:id="rId7"/>
+    <sheet name="2020 Child Count" sheetId="1" r:id="rId8"/>
+    <sheet name="2020 Census count" sheetId="2" r:id="rId9"/>
+    <sheet name="2020 census basic table for res" sheetId="6" r:id="rId10"/>
+    <sheet name="2020 % based on census" sheetId="3" r:id="rId11"/>
+    <sheet name="Oregon CC vs census " sheetId="5" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="74">
   <si>
     <t>State</t>
   </si>
@@ -269,6 +271,71 @@
   <si>
     <t>EI %</t>
   </si>
+  <si>
+    <r>
+      <t>Race/ethnicity Total</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (%)</t>
+    </r>
+  </si>
+  <si>
+    <t>American Indian or Alaska Native (%)</t>
+  </si>
+  <si>
+    <t>Asian (%)</t>
+  </si>
+  <si>
+    <t>Black or African American (%)</t>
+  </si>
+  <si>
+    <t>Hispanic/Latino (%)</t>
+  </si>
+  <si>
+    <t>Native Hawaiian or Pacific Islander (%)</t>
+  </si>
+  <si>
+    <t>Two or More Races (%)</t>
+  </si>
+  <si>
+    <t>White (%)</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Race/ethnicity Total3 (%)</t>
+  </si>
+  <si>
+    <r>
+      <t>Race/Ethnicity Total</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -277,7 +344,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -387,8 +454,55 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -419,8 +533,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -606,12 +726,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -872,10 +1004,76 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{8CE89FA7-92C8-AA49-9EE1-1799DC22FC18}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4843,6 +5041,988 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A374FE93-5A46-9E4D-82C9-F86D03222DFA}">
+  <dimension ref="A1:K34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H5" sqref="A1:H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+      <c r="A1" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="12">
+        <v>3735</v>
+      </c>
+      <c r="C2" s="13">
+        <v>2597</v>
+      </c>
+      <c r="D2" s="13">
+        <v>591</v>
+      </c>
+      <c r="E2" s="13">
+        <v>70</v>
+      </c>
+      <c r="F2" s="13">
+        <v>217</v>
+      </c>
+      <c r="G2" s="13">
+        <v>14</v>
+      </c>
+      <c r="H2" s="12">
+        <v>246</v>
+      </c>
+      <c r="I2" s="13">
+        <v>970</v>
+      </c>
+      <c r="J2" s="40">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="12">
+        <v>3774</v>
+      </c>
+      <c r="C3" s="13">
+        <v>2623</v>
+      </c>
+      <c r="D3" s="13">
+        <v>598</v>
+      </c>
+      <c r="E3" s="13">
+        <v>71</v>
+      </c>
+      <c r="F3" s="13">
+        <v>223</v>
+      </c>
+      <c r="G3" s="13">
+        <v>14</v>
+      </c>
+      <c r="H3" s="12">
+        <v>244</v>
+      </c>
+      <c r="I3" s="13">
+        <v>986</v>
+      </c>
+      <c r="J3" s="40">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="12">
+        <v>3853</v>
+      </c>
+      <c r="C4" s="13">
+        <v>2675</v>
+      </c>
+      <c r="D4" s="13">
+        <v>610</v>
+      </c>
+      <c r="E4" s="13">
+        <v>71</v>
+      </c>
+      <c r="F4" s="13">
+        <v>234</v>
+      </c>
+      <c r="G4" s="13">
+        <v>14</v>
+      </c>
+      <c r="H4" s="12">
+        <v>248</v>
+      </c>
+      <c r="I4" s="13">
+        <v>997</v>
+      </c>
+      <c r="J4" s="40">
+        <v>1859</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="39">
+        <v>11362</v>
+      </c>
+      <c r="C5" s="39">
+        <v>7895</v>
+      </c>
+      <c r="D5" s="39">
+        <v>1799</v>
+      </c>
+      <c r="E5" s="39">
+        <v>212</v>
+      </c>
+      <c r="F5" s="39">
+        <v>674</v>
+      </c>
+      <c r="G5" s="39">
+        <v>42</v>
+      </c>
+      <c r="H5" s="39">
+        <v>738</v>
+      </c>
+      <c r="I5" s="39">
+        <v>2953</v>
+      </c>
+      <c r="J5" s="41">
+        <v>5485</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="60" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="61" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="51">
+        <v>70</v>
+      </c>
+      <c r="C10" s="51">
+        <v>71</v>
+      </c>
+      <c r="D10" s="51">
+        <v>71</v>
+      </c>
+      <c r="E10" s="52">
+        <v>212</v>
+      </c>
+      <c r="F10" s="25">
+        <f>E10/E16</f>
+        <v>1.865868685090653E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="51">
+        <v>217</v>
+      </c>
+      <c r="C11" s="51">
+        <v>223</v>
+      </c>
+      <c r="D11" s="51">
+        <v>234</v>
+      </c>
+      <c r="E11" s="52">
+        <v>674</v>
+      </c>
+      <c r="F11" s="25">
+        <v>5.9320542158070762E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="51">
+        <v>591</v>
+      </c>
+      <c r="C12" s="51">
+        <v>598</v>
+      </c>
+      <c r="D12" s="51">
+        <v>610</v>
+      </c>
+      <c r="E12" s="52">
+        <v>1799</v>
+      </c>
+      <c r="F12" s="25">
+        <v>0.15833480021123042</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="51">
+        <v>14</v>
+      </c>
+      <c r="C13" s="51">
+        <v>14</v>
+      </c>
+      <c r="D13" s="51">
+        <v>14</v>
+      </c>
+      <c r="E13" s="52">
+        <v>42</v>
+      </c>
+      <c r="F13" s="25">
+        <v>3.696532300651294E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="51">
+        <v>246</v>
+      </c>
+      <c r="C14" s="51">
+        <v>244</v>
+      </c>
+      <c r="D14" s="51">
+        <v>248</v>
+      </c>
+      <c r="E14" s="52">
+        <v>738</v>
+      </c>
+      <c r="F14" s="25">
+        <v>6.4953353282872731E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="51">
+        <v>2597</v>
+      </c>
+      <c r="C15" s="51">
+        <v>2623</v>
+      </c>
+      <c r="D15" s="51">
+        <v>2675</v>
+      </c>
+      <c r="E15" s="52">
+        <v>7895</v>
+      </c>
+      <c r="F15" s="25">
+        <v>0.69486005984861821</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="51">
+        <v>3735</v>
+      </c>
+      <c r="C16" s="51">
+        <v>3774</v>
+      </c>
+      <c r="D16" s="51">
+        <v>3853</v>
+      </c>
+      <c r="E16" s="52">
+        <v>11362</v>
+      </c>
+      <c r="F16" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="51">
+        <v>970</v>
+      </c>
+      <c r="C17" s="51">
+        <v>986</v>
+      </c>
+      <c r="D17" s="51">
+        <v>997</v>
+      </c>
+      <c r="E17" s="52">
+        <v>2953</v>
+      </c>
+      <c r="F17" s="25">
+        <f>E17/E19</f>
+        <v>0.34996444655131548</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="51">
+        <v>1807</v>
+      </c>
+      <c r="C18" s="51">
+        <v>1819</v>
+      </c>
+      <c r="D18" s="51">
+        <v>1859</v>
+      </c>
+      <c r="E18" s="52">
+        <v>5485</v>
+      </c>
+      <c r="F18" s="25">
+        <f>E18/E19</f>
+        <v>0.65003555344868458</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="56">
+        <f>B17+B18</f>
+        <v>2777</v>
+      </c>
+      <c r="C19" s="56">
+        <f>C17+C18</f>
+        <v>2805</v>
+      </c>
+      <c r="D19" s="56">
+        <f>D17+D18</f>
+        <v>2856</v>
+      </c>
+      <c r="E19" s="57">
+        <f>E17+E18</f>
+        <v>8438</v>
+      </c>
+      <c r="F19" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="39"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="24"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="48"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="46"/>
+      <c r="K21" s="39"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE57A53-26B7-CD40-AFB1-B8A430F77433}">
+  <dimension ref="A1:M23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="56" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>1.4809640237513098E-2</v>
+      </c>
+      <c r="C2">
+        <v>4.7083478868319942E-2</v>
+      </c>
+      <c r="D2">
+        <v>0.12567237163814182</v>
+      </c>
+      <c r="E2">
+        <v>0.20628711142158576</v>
+      </c>
+      <c r="F2">
+        <v>2.9339853300733498E-3</v>
+      </c>
+      <c r="G2">
+        <v>5.1554313657003144E-2</v>
+      </c>
+      <c r="H2">
+        <v>0.55151938526021704</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>6.9348407491337388E-3</v>
+      </c>
+      <c r="C3">
+        <v>4.3881089204463847E-2</v>
+      </c>
+      <c r="D3">
+        <v>0.12350949000074785</v>
+      </c>
+      <c r="E3">
+        <v>0.27654962589608661</v>
+      </c>
+      <c r="F3">
+        <v>3.0353282772226926E-3</v>
+      </c>
+      <c r="G3">
+        <v>4.2318910083296433E-2</v>
+      </c>
+      <c r="H3">
+        <v>0.50377071578904886</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="91" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="94">
+        <v>2020</v>
+      </c>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="95"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="95"/>
+    </row>
+    <row r="8" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="92"/>
+      <c r="B8" s="96" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="94" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="98"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98"/>
+      <c r="H8" s="98"/>
+      <c r="I8" s="99"/>
+      <c r="J8" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="104" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+      <c r="A9" s="93"/>
+      <c r="B9" s="97"/>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="101"/>
+      <c r="K9" s="105"/>
+      <c r="L9" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="12">
+        <v>3735</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="13">
+        <v>2597</v>
+      </c>
+      <c r="E10" s="13">
+        <v>591</v>
+      </c>
+      <c r="F10" s="13">
+        <v>70</v>
+      </c>
+      <c r="G10" s="13">
+        <v>217</v>
+      </c>
+      <c r="H10" s="13">
+        <v>14</v>
+      </c>
+      <c r="I10" s="12">
+        <v>246</v>
+      </c>
+      <c r="J10" s="13">
+        <v>970</v>
+      </c>
+      <c r="K10" s="15">
+        <v>1807</v>
+      </c>
+      <c r="L10" s="5">
+        <f>SUM(J10:K10)</f>
+        <v>2777</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="12">
+        <v>3774</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="13">
+        <v>2623</v>
+      </c>
+      <c r="E11" s="13">
+        <v>598</v>
+      </c>
+      <c r="F11" s="13">
+        <v>71</v>
+      </c>
+      <c r="G11" s="13">
+        <v>223</v>
+      </c>
+      <c r="H11" s="13">
+        <v>14</v>
+      </c>
+      <c r="I11" s="12">
+        <v>244</v>
+      </c>
+      <c r="J11" s="13">
+        <v>986</v>
+      </c>
+      <c r="K11" s="15">
+        <v>1819</v>
+      </c>
+      <c r="L11" s="5">
+        <f t="shared" ref="L11:L12" si="0">SUM(J11:K11)</f>
+        <v>2805</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="12">
+        <v>3853</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="13">
+        <v>2675</v>
+      </c>
+      <c r="E12" s="13">
+        <v>610</v>
+      </c>
+      <c r="F12" s="13">
+        <v>71</v>
+      </c>
+      <c r="G12" s="13">
+        <v>234</v>
+      </c>
+      <c r="H12" s="13">
+        <v>14</v>
+      </c>
+      <c r="I12" s="12">
+        <v>248</v>
+      </c>
+      <c r="J12" s="13">
+        <v>997</v>
+      </c>
+      <c r="K12" s="15">
+        <v>1859</v>
+      </c>
+      <c r="L12" s="5">
+        <f t="shared" si="0"/>
+        <v>2856</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B13" s="5">
+        <f>SUM(B10:B12)</f>
+        <v>11362</v>
+      </c>
+      <c r="C13" s="5">
+        <v>19800</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" ref="D13:L13" si="1">SUM(D10:D12)</f>
+        <v>7895</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>1799</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="1"/>
+        <v>212</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="1"/>
+        <v>674</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" si="1"/>
+        <v>738</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" si="1"/>
+        <v>2953</v>
+      </c>
+      <c r="K13" s="16">
+        <f t="shared" si="1"/>
+        <v>5485</v>
+      </c>
+      <c r="L13" s="5">
+        <f t="shared" si="1"/>
+        <v>8438</v>
+      </c>
+      <c r="M13" s="5">
+        <f>SUM(B13+L13)</f>
+        <v>19800</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="5">
+        <v>5485</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="5">
+        <v>13380</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17">
+        <v>0.55151938526021704</v>
+      </c>
+      <c r="E16" s="17">
+        <f>E13/C13</f>
+        <v>9.0858585858585861E-2</v>
+      </c>
+      <c r="F16" s="17">
+        <f>F13/C13</f>
+        <v>1.0707070707070707E-2</v>
+      </c>
+      <c r="G16" s="17">
+        <f>G13/C13</f>
+        <v>3.4040404040404038E-2</v>
+      </c>
+      <c r="H16" s="17">
+        <f>H13/C13</f>
+        <v>2.1212121212121214E-3</v>
+      </c>
+      <c r="I16" s="17">
+        <f>I13/C13</f>
+        <v>3.727272727272727E-2</v>
+      </c>
+      <c r="J16" s="17">
+        <f>J13/C13</f>
+        <v>0.14914141414141413</v>
+      </c>
+      <c r="K16" s="17"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="21" spans="1:12" ht="56" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="6">
+        <v>842413</v>
+      </c>
+      <c r="C22" s="6">
+        <v>5842</v>
+      </c>
+      <c r="D22" s="6">
+        <v>36966</v>
+      </c>
+      <c r="E22" s="6">
+        <v>104046</v>
+      </c>
+      <c r="F22" s="6">
+        <v>232969</v>
+      </c>
+      <c r="G22" s="6">
+        <v>2557</v>
+      </c>
+      <c r="H22" s="6">
+        <v>35650</v>
+      </c>
+      <c r="I22" s="7">
+        <v>424383</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <f>C22/B22</f>
+        <v>6.9348407491337388E-3</v>
+      </c>
+      <c r="D23">
+        <f>D22/B22</f>
+        <v>4.3881089204463847E-2</v>
+      </c>
+      <c r="E23">
+        <f>E22/B22</f>
+        <v>0.12350949000074785</v>
+      </c>
+      <c r="F23">
+        <f>F22/B22</f>
+        <v>0.27654962589608661</v>
+      </c>
+      <c r="G23">
+        <f>G22/B22</f>
+        <v>3.0353282772226926E-3</v>
+      </c>
+      <c r="H23">
+        <f>H22/B22</f>
+        <v>4.2318910083296433E-2</v>
+      </c>
+      <c r="I23">
+        <f>I22/B22</f>
+        <v>0.50377071578904886</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="J8:J9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2803CB4-C907-A944-A2A7-4695A544927C}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -4943,6 +6123,220 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1FF994-930B-4842-9A20-6689702EFA99}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56C4A339-D70F-0E44-A0E8-2B7551E0CBD6}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="56" x14ac:dyDescent="0.2">
+      <c r="A1" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="107" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="108" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="107" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="107" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="108" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="107" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="107" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="113" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="114" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="115">
+        <v>9543</v>
+      </c>
+      <c r="C2" s="115">
+        <v>83</v>
+      </c>
+      <c r="D2" s="115">
+        <v>312</v>
+      </c>
+      <c r="E2" s="115">
+        <v>257</v>
+      </c>
+      <c r="F2" s="115">
+        <v>2173</v>
+      </c>
+      <c r="G2" s="115">
+        <v>29</v>
+      </c>
+      <c r="H2" s="115">
+        <v>516</v>
+      </c>
+      <c r="I2" s="116">
+        <v>6173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="112" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A3" s="109" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="110">
+        <v>100</v>
+      </c>
+      <c r="C3" s="111">
+        <v>0.87</v>
+      </c>
+      <c r="D3" s="110">
+        <v>3.27</v>
+      </c>
+      <c r="E3" s="110">
+        <v>2.69</v>
+      </c>
+      <c r="F3" s="110">
+        <v>22.77</v>
+      </c>
+      <c r="G3" s="110">
+        <v>0.3</v>
+      </c>
+      <c r="H3" s="110">
+        <v>5.41</v>
+      </c>
+      <c r="I3" s="110">
+        <v>64.69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="126" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="127" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="128" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="56" x14ac:dyDescent="0.2">
+      <c r="A7" s="125" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="117">
+        <v>83</v>
+      </c>
+      <c r="C7" s="118">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="124" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="117">
+        <v>312</v>
+      </c>
+      <c r="C8" s="119">
+        <v>3.27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="42" x14ac:dyDescent="0.2">
+      <c r="A9" s="124" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="117">
+        <v>257</v>
+      </c>
+      <c r="C9" s="119">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="28" x14ac:dyDescent="0.2">
+      <c r="A10" s="124" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="117">
+        <v>2173</v>
+      </c>
+      <c r="C10" s="119">
+        <v>22.77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="56" x14ac:dyDescent="0.2">
+      <c r="A11" s="125" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="117">
+        <v>29</v>
+      </c>
+      <c r="C11" s="119">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="28" x14ac:dyDescent="0.2">
+      <c r="A12" s="124" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="117">
+        <v>516</v>
+      </c>
+      <c r="C12" s="119">
+        <v>5.41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="124" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="120">
+        <v>6173</v>
+      </c>
+      <c r="C13" s="119">
+        <v>64.69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="123" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="121">
+        <v>9543</v>
+      </c>
+      <c r="C14" s="122">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB304EA7-6C1E-224C-AD55-AA784971FFF0}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4957,7 +6351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1A8275-12E4-4647-8849-23CE8825B359}">
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -5066,7 +6460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949D2739-F84A-4C43-9937-57F38C57A9F9}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -5150,11 +6544,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5136C5-25A9-8446-ABE1-D16B8F03F454}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" workbookViewId="0">
+    <sheetView topLeftCell="F16" workbookViewId="0">
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
@@ -5699,7 +7093,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92886FB8-A348-9B42-91B6-9401EDCBB5FB}">
   <dimension ref="A1:I14"/>
   <sheetViews>
@@ -5910,7 +7304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692B5770-BF87-E241-A98B-102B7F0055AF}">
   <dimension ref="A1:M9"/>
   <sheetViews>
@@ -6163,986 +7557,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A374FE93-5A46-9E4D-82C9-F86D03222DFA}">
-  <dimension ref="A1:K34"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H5" sqref="A1:H5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="102" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" s="45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="12">
-        <v>3735</v>
-      </c>
-      <c r="C2" s="13">
-        <v>2597</v>
-      </c>
-      <c r="D2" s="13">
-        <v>591</v>
-      </c>
-      <c r="E2" s="13">
-        <v>70</v>
-      </c>
-      <c r="F2" s="13">
-        <v>217</v>
-      </c>
-      <c r="G2" s="13">
-        <v>14</v>
-      </c>
-      <c r="H2" s="12">
-        <v>246</v>
-      </c>
-      <c r="I2" s="13">
-        <v>970</v>
-      </c>
-      <c r="J2" s="40">
-        <v>1807</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="12">
-        <v>3774</v>
-      </c>
-      <c r="C3" s="13">
-        <v>2623</v>
-      </c>
-      <c r="D3" s="13">
-        <v>598</v>
-      </c>
-      <c r="E3" s="13">
-        <v>71</v>
-      </c>
-      <c r="F3" s="13">
-        <v>223</v>
-      </c>
-      <c r="G3" s="13">
-        <v>14</v>
-      </c>
-      <c r="H3" s="12">
-        <v>244</v>
-      </c>
-      <c r="I3" s="13">
-        <v>986</v>
-      </c>
-      <c r="J3" s="40">
-        <v>1819</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="12">
-        <v>3853</v>
-      </c>
-      <c r="C4" s="13">
-        <v>2675</v>
-      </c>
-      <c r="D4" s="13">
-        <v>610</v>
-      </c>
-      <c r="E4" s="13">
-        <v>71</v>
-      </c>
-      <c r="F4" s="13">
-        <v>234</v>
-      </c>
-      <c r="G4" s="13">
-        <v>14</v>
-      </c>
-      <c r="H4" s="12">
-        <v>248</v>
-      </c>
-      <c r="I4" s="13">
-        <v>997</v>
-      </c>
-      <c r="J4" s="40">
-        <v>1859</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="39">
-        <v>11362</v>
-      </c>
-      <c r="C5" s="39">
-        <v>7895</v>
-      </c>
-      <c r="D5" s="39">
-        <v>1799</v>
-      </c>
-      <c r="E5" s="39">
-        <v>212</v>
-      </c>
-      <c r="F5" s="39">
-        <v>674</v>
-      </c>
-      <c r="G5" s="39">
-        <v>42</v>
-      </c>
-      <c r="H5" s="39">
-        <v>738</v>
-      </c>
-      <c r="I5" s="39">
-        <v>2953</v>
-      </c>
-      <c r="J5" s="41">
-        <v>5485</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="47" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="58" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="59" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="59" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="61" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="51">
-        <v>70</v>
-      </c>
-      <c r="C10" s="51">
-        <v>71</v>
-      </c>
-      <c r="D10" s="51">
-        <v>71</v>
-      </c>
-      <c r="E10" s="52">
-        <v>212</v>
-      </c>
-      <c r="F10" s="25">
-        <f>E10/E16</f>
-        <v>1.865868685090653E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="51">
-        <v>217</v>
-      </c>
-      <c r="C11" s="51">
-        <v>223</v>
-      </c>
-      <c r="D11" s="51">
-        <v>234</v>
-      </c>
-      <c r="E11" s="52">
-        <v>674</v>
-      </c>
-      <c r="F11" s="25">
-        <v>5.9320542158070762E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="51">
-        <v>591</v>
-      </c>
-      <c r="C12" s="51">
-        <v>598</v>
-      </c>
-      <c r="D12" s="51">
-        <v>610</v>
-      </c>
-      <c r="E12" s="52">
-        <v>1799</v>
-      </c>
-      <c r="F12" s="25">
-        <v>0.15833480021123042</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="49" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="51">
-        <v>14</v>
-      </c>
-      <c r="C13" s="51">
-        <v>14</v>
-      </c>
-      <c r="D13" s="51">
-        <v>14</v>
-      </c>
-      <c r="E13" s="52">
-        <v>42</v>
-      </c>
-      <c r="F13" s="25">
-        <v>3.696532300651294E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="51">
-        <v>246</v>
-      </c>
-      <c r="C14" s="51">
-        <v>244</v>
-      </c>
-      <c r="D14" s="51">
-        <v>248</v>
-      </c>
-      <c r="E14" s="52">
-        <v>738</v>
-      </c>
-      <c r="F14" s="25">
-        <v>6.4953353282872731E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="51">
-        <v>2597</v>
-      </c>
-      <c r="C15" s="51">
-        <v>2623</v>
-      </c>
-      <c r="D15" s="51">
-        <v>2675</v>
-      </c>
-      <c r="E15" s="52">
-        <v>7895</v>
-      </c>
-      <c r="F15" s="25">
-        <v>0.69486005984861821</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="51">
-        <v>3735</v>
-      </c>
-      <c r="C16" s="51">
-        <v>3774</v>
-      </c>
-      <c r="D16" s="51">
-        <v>3853</v>
-      </c>
-      <c r="E16" s="52">
-        <v>11362</v>
-      </c>
-      <c r="F16" s="54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="51">
-        <v>970</v>
-      </c>
-      <c r="C17" s="51">
-        <v>986</v>
-      </c>
-      <c r="D17" s="51">
-        <v>997</v>
-      </c>
-      <c r="E17" s="52">
-        <v>2953</v>
-      </c>
-      <c r="F17" s="25">
-        <f>E17/E19</f>
-        <v>0.34996444655131548</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="51">
-        <v>1807</v>
-      </c>
-      <c r="C18" s="51">
-        <v>1819</v>
-      </c>
-      <c r="D18" s="51">
-        <v>1859</v>
-      </c>
-      <c r="E18" s="52">
-        <v>5485</v>
-      </c>
-      <c r="F18" s="25">
-        <f>E18/E19</f>
-        <v>0.65003555344868458</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="56">
-        <f>B17+B18</f>
-        <v>2777</v>
-      </c>
-      <c r="C19" s="56">
-        <f>C17+C18</f>
-        <v>2805</v>
-      </c>
-      <c r="D19" s="56">
-        <f>D17+D18</f>
-        <v>2856</v>
-      </c>
-      <c r="E19" s="57">
-        <f>E17+E18</f>
-        <v>8438</v>
-      </c>
-      <c r="F19" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="39"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="24"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="46"/>
-      <c r="K21" s="39"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="48" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE57A53-26B7-CD40-AFB1-B8A430F77433}">
-  <dimension ref="A1:M23"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:K13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="56" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2">
-        <v>1.4809640237513098E-2</v>
-      </c>
-      <c r="C2">
-        <v>4.7083478868319942E-2</v>
-      </c>
-      <c r="D2">
-        <v>0.12567237163814182</v>
-      </c>
-      <c r="E2">
-        <v>0.20628711142158576</v>
-      </c>
-      <c r="F2">
-        <v>2.9339853300733498E-3</v>
-      </c>
-      <c r="G2">
-        <v>5.1554313657003144E-2</v>
-      </c>
-      <c r="H2">
-        <v>0.55151938526021704</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3">
-        <v>6.9348407491337388E-3</v>
-      </c>
-      <c r="C3">
-        <v>4.3881089204463847E-2</v>
-      </c>
-      <c r="D3">
-        <v>0.12350949000074785</v>
-      </c>
-      <c r="E3">
-        <v>0.27654962589608661</v>
-      </c>
-      <c r="F3">
-        <v>3.0353282772226926E-3</v>
-      </c>
-      <c r="G3">
-        <v>4.2318910083296433E-2</v>
-      </c>
-      <c r="H3">
-        <v>0.50377071578904886</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="91" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="94">
-        <v>2020</v>
-      </c>
-      <c r="C7" s="95"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="95"/>
-      <c r="I7" s="95"/>
-      <c r="J7" s="95"/>
-    </row>
-    <row r="8" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="92"/>
-      <c r="B8" s="96" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="94" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98"/>
-      <c r="H8" s="98"/>
-      <c r="I8" s="99"/>
-      <c r="J8" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="104" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="102" x14ac:dyDescent="0.2">
-      <c r="A9" s="93"/>
-      <c r="B9" s="97"/>
-      <c r="C9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="101"/>
-      <c r="K9" s="105"/>
-      <c r="L9" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="12">
-        <v>3735</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="13">
-        <v>2597</v>
-      </c>
-      <c r="E10" s="13">
-        <v>591</v>
-      </c>
-      <c r="F10" s="13">
-        <v>70</v>
-      </c>
-      <c r="G10" s="13">
-        <v>217</v>
-      </c>
-      <c r="H10" s="13">
-        <v>14</v>
-      </c>
-      <c r="I10" s="12">
-        <v>246</v>
-      </c>
-      <c r="J10" s="13">
-        <v>970</v>
-      </c>
-      <c r="K10" s="15">
-        <v>1807</v>
-      </c>
-      <c r="L10" s="5">
-        <f>SUM(J10:K10)</f>
-        <v>2777</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="12">
-        <v>3774</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="13">
-        <v>2623</v>
-      </c>
-      <c r="E11" s="13">
-        <v>598</v>
-      </c>
-      <c r="F11" s="13">
-        <v>71</v>
-      </c>
-      <c r="G11" s="13">
-        <v>223</v>
-      </c>
-      <c r="H11" s="13">
-        <v>14</v>
-      </c>
-      <c r="I11" s="12">
-        <v>244</v>
-      </c>
-      <c r="J11" s="13">
-        <v>986</v>
-      </c>
-      <c r="K11" s="15">
-        <v>1819</v>
-      </c>
-      <c r="L11" s="5">
-        <f t="shared" ref="L11:L12" si="0">SUM(J11:K11)</f>
-        <v>2805</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="12">
-        <v>3853</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="13">
-        <v>2675</v>
-      </c>
-      <c r="E12" s="13">
-        <v>610</v>
-      </c>
-      <c r="F12" s="13">
-        <v>71</v>
-      </c>
-      <c r="G12" s="13">
-        <v>234</v>
-      </c>
-      <c r="H12" s="13">
-        <v>14</v>
-      </c>
-      <c r="I12" s="12">
-        <v>248</v>
-      </c>
-      <c r="J12" s="13">
-        <v>997</v>
-      </c>
-      <c r="K12" s="15">
-        <v>1859</v>
-      </c>
-      <c r="L12" s="5">
-        <f t="shared" si="0"/>
-        <v>2856</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="5">
-        <f>SUM(B10:B12)</f>
-        <v>11362</v>
-      </c>
-      <c r="C13" s="5">
-        <v>19800</v>
-      </c>
-      <c r="D13" s="5">
-        <f t="shared" ref="D13:L13" si="1">SUM(D10:D12)</f>
-        <v>7895</v>
-      </c>
-      <c r="E13" s="5">
-        <f t="shared" si="1"/>
-        <v>1799</v>
-      </c>
-      <c r="F13" s="5">
-        <f t="shared" si="1"/>
-        <v>212</v>
-      </c>
-      <c r="G13" s="5">
-        <f t="shared" si="1"/>
-        <v>674</v>
-      </c>
-      <c r="H13" s="5">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-      <c r="I13" s="5">
-        <f t="shared" si="1"/>
-        <v>738</v>
-      </c>
-      <c r="J13" s="5">
-        <f t="shared" si="1"/>
-        <v>2953</v>
-      </c>
-      <c r="K13" s="16">
-        <f t="shared" si="1"/>
-        <v>5485</v>
-      </c>
-      <c r="L13" s="5">
-        <f t="shared" si="1"/>
-        <v>8438</v>
-      </c>
-      <c r="M13" s="5">
-        <f>SUM(B13+L13)</f>
-        <v>19800</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="5">
-        <v>5485</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="5">
-        <v>13380</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17">
-        <v>0.55151938526021704</v>
-      </c>
-      <c r="E16" s="17">
-        <f>E13/C13</f>
-        <v>9.0858585858585861E-2</v>
-      </c>
-      <c r="F16" s="17">
-        <f>F13/C13</f>
-        <v>1.0707070707070707E-2</v>
-      </c>
-      <c r="G16" s="17">
-        <f>G13/C13</f>
-        <v>3.4040404040404038E-2</v>
-      </c>
-      <c r="H16" s="17">
-        <f>H13/C13</f>
-        <v>2.1212121212121214E-3</v>
-      </c>
-      <c r="I16" s="17">
-        <f>I13/C13</f>
-        <v>3.727272727272727E-2</v>
-      </c>
-      <c r="J16" s="17">
-        <f>J13/C13</f>
-        <v>0.14914141414141413</v>
-      </c>
-      <c r="K16" s="17"/>
-      <c r="L16" s="5"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-    </row>
-    <row r="21" spans="1:12" ht="56" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="6">
-        <v>842413</v>
-      </c>
-      <c r="C22" s="6">
-        <v>5842</v>
-      </c>
-      <c r="D22" s="6">
-        <v>36966</v>
-      </c>
-      <c r="E22" s="6">
-        <v>104046</v>
-      </c>
-      <c r="F22" s="6">
-        <v>232969</v>
-      </c>
-      <c r="G22" s="6">
-        <v>2557</v>
-      </c>
-      <c r="H22" s="6">
-        <v>35650</v>
-      </c>
-      <c r="I22" s="7">
-        <v>424383</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C23">
-        <f>C22/B22</f>
-        <v>6.9348407491337388E-3</v>
-      </c>
-      <c r="D23">
-        <f>D22/B22</f>
-        <v>4.3881089204463847E-2</v>
-      </c>
-      <c r="E23">
-        <f>E22/B22</f>
-        <v>0.12350949000074785</v>
-      </c>
-      <c r="F23">
-        <f>F22/B22</f>
-        <v>0.27654962589608661</v>
-      </c>
-      <c r="G23">
-        <f>G22/B22</f>
-        <v>3.0353282772226926E-3</v>
-      </c>
-      <c r="H23">
-        <f>H22/B22</f>
-        <v>4.2318910083296433E-2</v>
-      </c>
-      <c r="I23">
-        <f>I22/B22</f>
-        <v>0.50377071578904886</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="J8:J9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>